<commit_message>
Partial changes - not getting all records
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -1,27 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\ZIMS_enrichmentReader\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E7E7755-69B3-4F92-A3E6-028E78CC9F49}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Data" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1084" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1277" uniqueCount="208">
   <si>
     <t>individual</t>
   </si>
@@ -80,31 +73,34 @@
     <t>details</t>
   </si>
   <si>
-    <t>GAN:MIG12-29698271 / Alive / Male  / -</t>
-  </si>
-  <si>
-    <t>[040015/BARABOO][215977/NZP-WASH]</t>
-  </si>
-  <si>
-    <t>KITO</t>
-  </si>
-  <si>
-    <t>Anthropoides paradiseus / Stanley crane   IUCN : VUCITES : II</t>
-  </si>
-  <si>
-    <t>Smithsonian National Zoological Park</t>
+    <t>GAN:MIG12-7509000 / Alive / Female  / -</t>
+  </si>
+  <si>
+    <t>[020026/BARABOO][010034/WORLDBIRD]</t>
+  </si>
+  <si>
+    <t>Slidell</t>
+  </si>
+  <si>
+    <t>Balearica regulorum gibbericeps / East African grey crowned-crane   IUCN : ENCITES : II</t>
+  </si>
+  <si>
+    <t>Private Collection</t>
   </si>
   <si>
     <t>Captive Birth/Hatch</t>
   </si>
   <si>
-    <t xml:space="preserve">May 23, 2011 / 8 Years 7 Months 29 Days </t>
+    <t xml:space="preserve">Jun 14, 2001 / 18 Years 7 Months 20 Days </t>
   </si>
   <si>
     <t>Main Institution Animal Collection</t>
   </si>
   <si>
-    <t>CC 1 AB</t>
+    <t>CC 58 AB</t>
+  </si>
+  <si>
+    <t>Occupational</t>
   </si>
   <si>
     <t>Environmental</t>
@@ -116,12 +112,87 @@
     <t>Food</t>
   </si>
   <si>
-    <t>Occupational</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
+    <t>Nov 25, 2019</t>
+  </si>
+  <si>
+    <t>Nov 26, 2019</t>
+  </si>
+  <si>
+    <t>Nov 27, 2019</t>
+  </si>
+  <si>
+    <t>Dec 02, 2019</t>
+  </si>
+  <si>
+    <t>Dec 04, 2019</t>
+  </si>
+  <si>
+    <t>Dec 06, 2019</t>
+  </si>
+  <si>
+    <t>Dec 08, 2019</t>
+  </si>
+  <si>
+    <t>Dec 09, 2019</t>
+  </si>
+  <si>
+    <t>Dec 11, 2019</t>
+  </si>
+  <si>
+    <t>Dec 18, 2019</t>
+  </si>
+  <si>
+    <t>Dec 19, 2019</t>
+  </si>
+  <si>
+    <t>Dec 23, 2019</t>
+  </si>
+  <si>
+    <t>Dec 24, 2019</t>
+  </si>
+  <si>
+    <t>Dec 30, 2019</t>
+  </si>
+  <si>
+    <t>Jan 06, 2020</t>
+  </si>
+  <si>
+    <t>Jan 07, 2020</t>
+  </si>
+  <si>
+    <t>Jan 08, 2020</t>
+  </si>
+  <si>
+    <t>Jan 11, 2020</t>
+  </si>
+  <si>
+    <t>Jan 13, 2020</t>
+  </si>
+  <si>
+    <t>Jan 20, 2020</t>
+  </si>
+  <si>
+    <t>Jan 22, 2020</t>
+  </si>
+  <si>
+    <t>Jan 26, 2020</t>
+  </si>
+  <si>
+    <t>Jan 27, 2020</t>
+  </si>
+  <si>
+    <t>Jan 28, 2020</t>
+  </si>
+  <si>
+    <t>Jan 29, 2020</t>
+  </si>
+  <si>
+    <t>Feb 03, 2020</t>
+  </si>
+  <si>
     <t>Nov 24, 2019</t>
   </si>
   <si>
@@ -134,16 +205,13 @@
     <t>Dec 05, 2019</t>
   </si>
   <si>
-    <t>Dec 08, 2019</t>
-  </si>
-  <si>
     <t>Dec 12, 2019</t>
   </si>
   <si>
     <t>Dec 15, 2019</t>
   </si>
   <si>
-    <t>Dec 19, 2019</t>
+    <t>Dec 16, 2019</t>
   </si>
   <si>
     <t>Dec 22, 2019</t>
@@ -152,515 +220,562 @@
     <t>Dec 26, 2019</t>
   </si>
   <si>
+    <t>Jan 02, 2020</t>
+  </si>
+  <si>
+    <t>Jan 05, 2020</t>
+  </si>
+  <si>
+    <t>Jan 09, 2020</t>
+  </si>
+  <si>
+    <t>Jan 10, 2020</t>
+  </si>
+  <si>
+    <t>Jan 12, 2020</t>
+  </si>
+  <si>
+    <t>Jan 15, 2020</t>
+  </si>
+  <si>
+    <t>Jan 16, 2020</t>
+  </si>
+  <si>
+    <t>Jan 19, 2020</t>
+  </si>
+  <si>
+    <t>Jan 23, 2020</t>
+  </si>
+  <si>
+    <t>Jan 30, 2020</t>
+  </si>
+  <si>
+    <t>Feb 02, 2020</t>
+  </si>
+  <si>
+    <t>Nov 22, 2019</t>
+  </si>
+  <si>
+    <t>Nov 29, 2019</t>
+  </si>
+  <si>
+    <t>Dec 20, 2019</t>
+  </si>
+  <si>
+    <t>Dec 27, 2019</t>
+  </si>
+  <si>
+    <t>Jan 03, 2020</t>
+  </si>
+  <si>
+    <t>Jan 17, 2020</t>
+  </si>
+  <si>
+    <t>Jan 24, 2020</t>
+  </si>
+  <si>
+    <t>Jan 31, 2020</t>
+  </si>
+  <si>
+    <t>Nov 23, 2019</t>
+  </si>
+  <si>
+    <t>Nov 30, 2019</t>
+  </si>
+  <si>
+    <t>Dec 03, 2019</t>
+  </si>
+  <si>
+    <t>Dec 07, 2019</t>
+  </si>
+  <si>
+    <t>Dec 10, 2019</t>
+  </si>
+  <si>
+    <t>Dec 13, 2019</t>
+  </si>
+  <si>
+    <t>Dec 14, 2019</t>
+  </si>
+  <si>
+    <t>Dec 17, 2019</t>
+  </si>
+  <si>
+    <t>Dec 21, 2019</t>
+  </si>
+  <si>
+    <t>Dec 28, 2019</t>
+  </si>
+  <si>
     <t>Dec 29, 2019</t>
   </si>
   <si>
-    <t>Dec 30, 2019</t>
-  </si>
-  <si>
-    <t>Jan 02, 2020</t>
-  </si>
-  <si>
-    <t>Jan 05, 2020</t>
-  </si>
-  <si>
-    <t>Jan 09, 2020</t>
-  </si>
-  <si>
-    <t>Jan 10, 2020</t>
-  </si>
-  <si>
-    <t>Jan 12, 2020</t>
-  </si>
-  <si>
-    <t>Jan 16, 2020</t>
-  </si>
-  <si>
-    <t>Jan 19, 2020</t>
-  </si>
-  <si>
-    <t>Nov 22, 2019</t>
-  </si>
-  <si>
-    <t>Nov 29, 2019</t>
-  </si>
-  <si>
-    <t>Dec 06, 2019</t>
-  </si>
-  <si>
-    <t>Dec 13, 2019</t>
-  </si>
-  <si>
-    <t>Dec 20, 2019</t>
-  </si>
-  <si>
-    <t>Dec 27, 2019</t>
-  </si>
-  <si>
-    <t>Jan 03, 2020</t>
-  </si>
-  <si>
-    <t>Jan 17, 2020</t>
-  </si>
-  <si>
-    <t>Nov 23, 2019</t>
-  </si>
-  <si>
-    <t>Nov 30, 2019</t>
-  </si>
-  <si>
-    <t>Dec 03, 2019</t>
-  </si>
-  <si>
-    <t>Dec 07, 2019</t>
-  </si>
-  <si>
-    <t>Dec 10, 2019</t>
-  </si>
-  <si>
-    <t>Dec 14, 2019</t>
-  </si>
-  <si>
-    <t>Dec 21, 2019</t>
-  </si>
-  <si>
-    <t>Dec 28, 2019</t>
-  </si>
-  <si>
     <t>Dec 31, 2019</t>
   </si>
   <si>
     <t>Jan 04, 2020</t>
   </si>
   <si>
-    <t>Jan 11, 2020</t>
-  </si>
-  <si>
     <t>Jan 14, 2020</t>
   </si>
   <si>
     <t>Jan 18, 2020</t>
   </si>
   <si>
-    <t>Nov 25, 2019</t>
-  </si>
-  <si>
-    <t>Nov 26, 2019</t>
-  </si>
-  <si>
-    <t>Nov 27, 2019</t>
-  </si>
-  <si>
-    <t>Dec 02, 2019</t>
-  </si>
-  <si>
-    <t>Dec 04, 2019</t>
-  </si>
-  <si>
-    <t>Dec 09, 2019</t>
-  </si>
-  <si>
-    <t>Dec 11, 2019</t>
-  </si>
-  <si>
-    <t>Dec 16, 2019</t>
-  </si>
-  <si>
-    <t>Dec 17, 2019</t>
-  </si>
-  <si>
-    <t>Dec 18, 2019</t>
-  </si>
-  <si>
-    <t>Dec 23, 2019</t>
-  </si>
-  <si>
-    <t>Dec 24, 2019</t>
-  </si>
-  <si>
-    <t>Jan 01, 2020</t>
-  </si>
-  <si>
-    <t>Jan 06, 2020</t>
-  </si>
-  <si>
-    <t>Jan 07, 2020</t>
-  </si>
-  <si>
-    <t>Jan 08, 2020</t>
-  </si>
-  <si>
-    <t>Jan 13, 2020</t>
-  </si>
-  <si>
-    <t>Jan 15, 2020</t>
-  </si>
-  <si>
-    <t>Jan 20, 2020</t>
-  </si>
-  <si>
-    <t>08:30:00</t>
-  </si>
-  <si>
-    <t>08:45:00</t>
+    <t>Jan 21, 2020</t>
+  </si>
+  <si>
+    <t>Jan 25, 2020</t>
+  </si>
+  <si>
+    <t>Feb 01, 2020</t>
+  </si>
+  <si>
+    <t>10:30:00</t>
+  </si>
+  <si>
+    <t>10:00:00</t>
+  </si>
+  <si>
+    <t>09:45:00</t>
+  </si>
+  <si>
+    <t>11:15:00</t>
+  </si>
+  <si>
+    <t>11:00:00</t>
+  </si>
+  <si>
+    <t>10:45:00</t>
   </si>
   <si>
     <t>09:00:00</t>
   </si>
   <si>
-    <t>10:45:00</t>
+    <t>Not Observed</t>
+  </si>
+  <si>
+    <t>Evaluation neutral</t>
+  </si>
+  <si>
+    <t>Positive</t>
+  </si>
+  <si>
+    <t>Neutral</t>
   </si>
   <si>
     <t>Evaluation positive</t>
   </si>
   <si>
-    <t>Not Observed</t>
-  </si>
-  <si>
-    <t>Evaluation neutral</t>
-  </si>
-  <si>
-    <t>Positive</t>
-  </si>
-  <si>
-    <t>Neutral</t>
+    <t>Evaluation negative</t>
+  </si>
+  <si>
+    <t>Ignored item</t>
+  </si>
+  <si>
+    <t>Moderately Successful</t>
   </si>
   <si>
     <t>Highly Successful</t>
   </si>
   <si>
-    <t>Moderately Successful</t>
+    <t>No Reaction</t>
+  </si>
+  <si>
+    <t>Moderately Unsuccessful</t>
   </si>
   <si>
     <t>Highly Unsuccessful</t>
   </si>
   <si>
+    <t>Cynthia Gitter</t>
+  </si>
+  <si>
+    <t>Allyce Vogel, Cynthia Gitter</t>
+  </si>
+  <si>
+    <t>Allyce Vogel</t>
+  </si>
+  <si>
+    <t>Andrew Craton</t>
+  </si>
+  <si>
+    <t>Zach Zeillmann</t>
+  </si>
+  <si>
+    <t>Taylor Ennis</t>
+  </si>
+  <si>
+    <t>Kim Boardman</t>
+  </si>
+  <si>
+    <t>Kyle Tainter</t>
+  </si>
+  <si>
     <t>Maggie Bednarek</t>
   </si>
   <si>
-    <t>Allyce Vogel</t>
-  </si>
-  <si>
-    <t>Cynthia Gitter</t>
-  </si>
-  <si>
-    <t>Taylor Ennis</t>
+    <t>Jessica Colvin</t>
   </si>
   <si>
     <t>Marianne Wellington</t>
   </si>
   <si>
-    <t>Allyce Vogel, Cynthia Gitter</t>
-  </si>
-  <si>
-    <t>Kyle Tainter</t>
-  </si>
-  <si>
-    <t>Jessica Colvin</t>
-  </si>
-  <si>
-    <t>Kim Boardman</t>
-  </si>
-  <si>
-    <t>2x treat bowl with bark chips, 3 clementine wedges and field corn.
-Bowls were empty &amp; one was flipped upside down when removed at CC check. KB</t>
-  </si>
-  <si>
-    <t>(2) treat bowl with water, lettuce and cranberries. Will be left with them overnight.
-Removed: 11/29 ~0900
-Eval:  Some lettuce and crans out of bowl, water spilled. Extreme interest. MB</t>
-  </si>
-  <si>
-    <t>(2) treat bowls with top soil, mealworms buried, and 2 green grapes on top. Placed bowls in center section of house, since no camera up to watch interaction.
-Removed: 12/1 pm, MB
-Eval: Grapes and mlws gone, some dirt pulled out of bowl. Extreme interest</t>
-  </si>
-  <si>
-    <t>2x treat bowl with water, half pumpkin and a sprinkle of cabbage.
-Removed: AV 12/5 15:00
-Eval: Extreme interest. The pumpkins had dozens of peck marks in them, water was spilled/splashed outside onto the shavings. I didn't find any cabbage.</t>
-  </si>
-  <si>
-    <t>2x treat bowl with a few river rocks, corn, peanuts and dried leaves.
-Removed: TE removed during PM check. Some leaves had been picked out and peanuts were gone. 
-Eval: Moderate interest</t>
-  </si>
-  <si>
-    <t>(2) treat bowl of planted grass seed, grown up above the rim of the bowl. a few mealworms on top.
+    <t>Crane Conservation Department</t>
+  </si>
+  <si>
+    <t>Treat bowl with pumpkin half, shredded paper and mealworms placed inside house. 
+Date Removed: 11/25 by AV
+Evaluation: Ate the mealworms, but otherwise did not appear to do much with the pumpkin or paper.</t>
+  </si>
+  <si>
+    <t>Treat bowl with bark chips and the top of a red pepper with seeds. Mealworms were hidden amongst the bark chips. Left the bowl in front section of her house.
+Date removed: 26 Nov
+Evaluation:  Moderate interest; mealworms gone, bark chips played in, pepper untouched - CG</t>
+  </si>
+  <si>
+    <t>Treat bowl with top soil and blue kong with mealworms inside, came over and was investigating right away.
+Removed: 11/27 @ 1600
+Eval: Ball still in bowl, g pep still in ball. Some mlws left in soil, some soil spilled out of bowl. Moderate interest. MB</t>
+  </si>
+  <si>
+    <t>Placed small treat bowl with bark chips and pomegranate seeds in back of house. (Did not see any enrichment to remove.) 
+Removed at PM CC check and seeds were mostly gone, and bark had been tossed out of bowl.</t>
+  </si>
+  <si>
+    <t>small treat bowl with water, lettuce and some mealworms.
+Removed:
+Eval: Slidell went over and drank some water from the bowl right away.</t>
+  </si>
+  <si>
+    <t>Hollow toy ball filled w/ two grapes, three crane feathers. No clear signs of interaction.</t>
+  </si>
+  <si>
+    <t>Small treat bowl with leaves, river rocks, peanuts, and corn given inside house. Slidell walked up the dish right away and starting interacting with it. 
+Removed: TE removed during PM CC check. Some leaves and rocks had been removed but corn was still present. Did not see any peanuts.
+Evaluation: Moderate interest</t>
+  </si>
+  <si>
+    <t>Treat bowl with 1/2 cored apple, mealworms, and leaves on top placed in front of house. 
+Removed by &amp; date: Zach Zeillmann, 12/9/2019
+Evaluation: Extreme interest, all items except for 1 leaf removed from bowl, mlws eaten, apple removed but had few signs of interaction.</t>
+  </si>
+  <si>
+    <t>Treat bowl with the large Holy roller ball stuffed with straw and 3 in-shell peanuts. She came over and looked at it right away, but then was too preoccupied with me being there.
+Removed: 12/11
+Eval: All peanuts remained, but some straw had maybe been pulled out of the ball.</t>
+  </si>
+  <si>
+    <t>Enrichment given:  Treat bowl with dirt, mealworms, peanuts, straw placed in house.
+Date/Time removed: 12/18 PM by MB
+Evaluation: Straw pulled out, no treats leftover, some dirt spilled out of bowl. Extreme interest</t>
+  </si>
+  <si>
+    <t>Enrichment given:  Treat bowl with mealworms, corn, rock, and shredded paper placed inside house.
+Removed:  KT, 19 Dem PM
+Eval:  Few pieces of paper in shavings.  Mealworms gone but few pieces of corn remained.</t>
+  </si>
+  <si>
+    <t>Small treat bowl with mealworms, clementine wedges, and shredded newspaper on top placed inside first half of house. 
+Removed by &amp; date:  23 Dec PM
+Eval:  No interest; untouched</t>
+  </si>
+  <si>
+    <t>Treat bowl in house with leaves, mulch, and blueberries.</t>
+  </si>
+  <si>
+    <t>treat bowl of bark chips with pomegranate seeds hidden.
+Removed: 12/30 AV
+Eval: I found a couple pom seeds that she hadnn't found in the bowl yet, but she found and ate most of them, and many bark chips were scattered in the shavings.</t>
+  </si>
+  <si>
+    <t>PVC treat dispenser with mealworms inside placed in first half of house. 
+Date/time removed: 6 Jan PM
+Eval:  No interest, appeared untouched.</t>
+  </si>
+  <si>
+    <t>Small treatbowl with cranberries, mealworms and oak leaves placed inside house.
+Removed: 7 Jan, KT
+Eval: Looked to be untouched by PM check.</t>
+  </si>
+  <si>
+    <t>Small treat bowl with bark chips, mealworms, and corn placed in first half of house. 
+Date/time removed: 1/8 during PM CC check.
+Eval: Moderate interest. A few pieces of the bark chips had been removed and mealworms appeared to have been eaten.</t>
+  </si>
+  <si>
+    <t>Small treat bowl, mlws, baby peppers, and lettuce, with a bit of water in bowl. Place in NW corner on S side of house. 
+Removed:Check 11 jan 2020
+Eval: slightly interested.  1 pepper outside bowl, no mealworms found. Lettuce &amp; other peppers still in bowl.</t>
+  </si>
+  <si>
+    <t>Small treat bowl with a quarter chunk of pomegranite and leaves on top placed in first half of house. 
+Date/time removed: 1/13 AV
+Eval: Bowl was flipped, pom looked untouched.</t>
+  </si>
+  <si>
+    <t>Paper lunch bag (cut short) with top soil, some seeds and mealworms on top. Then 3 piecesof newspaper fitted into slits in the paper bag going across the top of it.
+Removed:1/20 AV
+Eval: Dumped the bag over and newspaper was outl. No evidence of treats.</t>
+  </si>
+  <si>
+    <t>Treat bowl with bark chips, 2 treat gelatin cubes, 2 peanuts and leaves over the top
+Removed:  22 Jan CG
+Eval:   Moderate interest; peanuts gone, few leaves outside bowl, rest looked untouched.</t>
+  </si>
+  <si>
+    <t>Description/ placement: treat bowl with bark chips, clementine wedges and blueberries covered with evergreen branches. Placed on E side of house
+Removed date/initials: 1/26 AV
+Evaluation: Untouched</t>
+  </si>
+  <si>
+    <t>Description/ placement: lettuce and water in small treat bowl with some mealworms. Placed in the house.
+Removed date/initials: 1/27 TE
+Evaluation: Extreme interest. Lettuce was all pulled out of bowl and water &amp; mealworms were gone.</t>
+  </si>
+  <si>
+    <t>Description/ placement:  Treat bowl with treats &amp; bark.
+Removed date/initials: 28 Jan CG
+Evaluation:  Moderate interest; treats gone, bark somewhat scattered.</t>
+  </si>
+  <si>
+    <t>Description/ placement: Hol-ee roller ball stuffed with straw and 4 mealworms inside. Placed it inside a treat bowl.
+Removed date/initials: 29 Jan MB
+Evaluation: All straw still in ball, couldn't see mlws but might've been in shavings or center of ball. No interest</t>
+  </si>
+  <si>
+    <t>Description/ placement: cored and scored apple with sprouted seeds and mealworms inside
+Removed date/initials:
+Evaluation:</t>
+  </si>
+  <si>
+    <t>Small treat bowl of bark chips with some field corn hidden. Was digging in the bowl right away after I put it down.
+Date Removed:  25 Nov 2019
+Evaluation:  Extreme interest; corn gone and bark tossed everywhere. CG</t>
+  </si>
+  <si>
+    <t>Treat bowl with cranberries and lettuce placed in house.
+Removed: 11/29 1000
+Evaluation: Most lettuce and crans left in bowl. No interest. MB</t>
+  </si>
+  <si>
+    <t>1 small treat bowl of dirt with mealworms and 2 green grapes on top.
+Removed: 12/1 pm, MB
+Eval: Grapes and mlws gone, lots of dirt out of bowl. Extreme interest</t>
+  </si>
+  <si>
+    <t>small treat bowl ice cubes with cranberry, peas and leaves on top.
+Removed: Everything tossed out of bowl, leaves everywhere -JC
+Eval: Successful</t>
+  </si>
+  <si>
+    <t>Grass treat bowl with a few mlws placed on W side of house
 Removed:12/12 AV
-Eval: DESTROYED. pulled a lot of the grass completely out of the footbath. no mealworms.</t>
-  </si>
-  <si>
-    <t>2x treat bowl with water, peas, 2 treat ice cubes, 2 leaves
-Removed: 12/15 in PM by JC
-Eval: found some smashed ice in bowl and around bowl, but all treats gone, leaves out of bowls.</t>
-  </si>
-  <si>
-    <t>2x treat bowl with newspaper shreds, 1 gelatin treat cube, some corn and a couple rocks
-removed: Kt, Dec 19 PM
-Eval: Paper shreds tossed around in shavings, gelatin cube picked apart and corn gone.</t>
-  </si>
-  <si>
-    <t>Enrichment given:  2 treat bowls with mealwomrs, 2 clementine pieces and lettuce.
-Date/Time removed: TE removed 12/22 during PM check.
-Evaluation: Moderate interest. Much of the lettuce had been taken out of one dish and most of the treats were gone.</t>
-  </si>
-  <si>
-    <t>(2) treat bowl with straw, cranberries, mealworms.
-Removed:26 Dec 2019
-Eval:straw was strewn around outside of the bowls and both cranberries and mealworms were missing.</t>
-  </si>
-  <si>
-    <t>(2) treat bowl with small pieces of sweet potatoe and some slices of regular potato in water with ~ 8 mealworms.
-Removed: 12/29 by MB
-Eval: mlws and potato gone, water dirty and still had sweet potato</t>
-  </si>
-  <si>
-    <t>Two small treat bowls with bark chips and pomegranite seeds placed in East section of house. 
-Removed: 12/30 AV
-Eval: No pomegranate seeds remained and bark chips scattered everywhere.</t>
-  </si>
-  <si>
-    <t>2x grass footbaths with some mlws
-Removed:  2 jan 2020 pm, MW
-Eval:extremely interested. Grass and soil pulled out of bowls, didn't see mealworms.</t>
-  </si>
-  <si>
-    <t>(2) treat bowl with pieces of coniferr branches, apple, cranberry, and a couple mealworms.
-Removed: 1/5/20 AV
-Eval: Every conifer branch piece had been removed from bowl and every treat was gone.</t>
-  </si>
-  <si>
-    <t>Placed 2 bowls of pomegranite arials, mealworms covered wiith straw.
+Eval: DESTROYED. Hardly any grass left in the footbath and a bunch of dirt had been flung around as well.</t>
+  </si>
+  <si>
+    <t>Small treat bowl with peas, ice cubes w/ frozen treats, leaves, and water placed inside first half of house. 
+Removed by and date: 12/15 Pm by JC
+Eval: *started to interact w/ water &amp; leaves right away.* **all treats gone, a little water in bowl**</t>
+  </si>
+  <si>
+    <t>Enrichment given:  Treat bowl with 1/2 head lettuce with corn, mealworms stuck in it placed in house. 
+Date/Time removed: TE removed on 12/16 during PM CC check.
+Evaluation: Extreme interest. Entire 1/2 head of lettuce taken out of bowl and pecked at. A few treats (corn) remained but most were eaten.</t>
+  </si>
+  <si>
+    <t>Small treat bowl with mealworms, two clementine slices, and lettuce placed inside first section of house.
+Removed: TE removed during PM check. 
+Eval: Moderate interest. Some lettuce had been pecked at, clementine slices remained, and mealworms gone.</t>
+  </si>
+  <si>
+    <t>Treat bowl with hay, cranberries, mlw placed on W side of house.
+Removed: 12/26 AV
+Eval: Looked untouched.</t>
+  </si>
+  <si>
+    <t>Small grass footbath with some mealworms.
+Removed:2 Jan 2020, MW
+Eval: Extremely interested. Grass/soil outside of bowl, no mealworms seen.</t>
+  </si>
+  <si>
+    <t>Enrichment given:  Treat bowl with cranberries, apple chunks, mealworms and evergreen boughs placed in house. 
+Date/Time removed: 1/5/20 16:00 AV
+Evaluation: No interest</t>
+  </si>
+  <si>
+    <t>Gave a bowl of mealworms, pomegranite arials covered w/straw.
 Removed: 1/9 PM, MB
-Eval: All treats gone, straw pulled out of bowl and scattered around</t>
-  </si>
-  <si>
-    <t>Gave 2 small footbaths with ripped paper, rocks blueberries &amp; mealworms in it on the east side.
-Removed: 1/10 Pm JC
-Eval: some newspaper out of 1 bowl, bluberries and mlws gone</t>
-  </si>
-  <si>
-    <t>2x treat bowl with evergreen branches, pomegranate seeds and cranberries
-Removed: 1/12 PM by MB
-Eval: Branches out of bowls, one bowl flipped over. Most treats eaten, saw a couple pom seeds and a cran leftover but that's it</t>
-  </si>
-  <si>
-    <t>(2) treat bowls planted with grass. mealworms and blueberries on top.</t>
-  </si>
-  <si>
-    <t>Placed 2 small bowls of soil/grass on the east end of the house.</t>
-  </si>
-  <si>
-    <t>(2) small treat bowls with bark chips, 2 grapes, mealworms, and covered with pieces of fir branches.
-Removed: 1/19 AV
-Eval: All the fir pieces were thrown out of the bowl, the majority of the bark chips were also spilled. No grapes or mealworms found.</t>
-  </si>
-  <si>
-    <t>2x treat bowl with 2 gelatin treat cubes (blueberry, peanut, dried mlws), a couple of ripped leaves and a couple inches of water.
-PM: removed bowl.  Moderate interest.  Gelatin had been removed from both bowls.  One  gelatin block was in pieces, peanut, blueberries and mealworms present.  Other gelatin block was whole.  A few leaves were outside the bowl.
-This note added to the following animals: 040016, 040015</t>
-  </si>
-  <si>
-    <t xml:space="preserve">
-2x treat bowl with newspaper strips, mlws and 3 clementine wedges.
-Removed: Zach Zeillmann
-Eval: All mlws eaten, clementines removed, some newspaper removed</t>
-  </si>
-  <si>
-    <t>2x treat bowl with 1/2 large treat gelatin circle (from blue mlw container). Newspaper shreds on top. **Only one newspaper shred removed, no further signs of interaction.</t>
-  </si>
-  <si>
-    <t>2x treat bowl with water, big pieces of lettuce, and apple slices.
-Removed: 13 Dec PM, KT
-Eval: One bowl still had quite a bit of water in it but the other mst have been tipped over since no water in it.  Lettuce still remained but apple slices gone.</t>
-  </si>
-  <si>
-    <t>2x treat bowl with water, treat ice cube, 3 blueberries and some lettuce
-removed: 12/20 PM by MB
-EVal: lettuce scattered, blueberries smashed</t>
-  </si>
-  <si>
-    <t>2x treat bowl with 2 rocks, dried mlw, lettuce, a clem wedge and some water
-Removed: 12/27 PM by MB
-Eval: Treats gone, lettuce scattered</t>
-  </si>
-  <si>
-    <t>2x treat bowl with water, dried leaves, brussel sprouts and pomegranate seeds
-Removed: 1/3 PM by MB
-Eval: Brussel sprouts picked apart a bit, one pulled out of bowl but rest still in bowl. Leaves still in bowl, pom seeds gone</t>
-  </si>
-  <si>
-    <t>2x treat bowl with ~1inch of water, evergreen branches, 2 clementine slices and dried mlws
-Removed: 17 Jan, KT
-Eval: Clementine slices and mealworms gone.  Evergreen branches laying in shavings.</t>
-  </si>
-  <si>
-    <t>Placed two treat bowls in the East side of the house that contained lettuce, pair slices, and clementine wedges. **Removed by ZZ ~1645. Removed bowls stuff tossed out of bowl**</t>
-  </si>
-  <si>
-    <t>2x treat bowl with lettuce, small squash slices, 1 pear slice and a few peanuts.
-Removed:
-Evaluation:</t>
-  </si>
-  <si>
-    <t>(2) treat bowl with pieces of yellow squash (yellow zucchini), pomegranate seeds, and 4 clementine wedges covered by a few leaves.
-Removed: AV 12/3
-Eval: Every food item had been eaten and the leaves were mostly outside the bowl.</t>
-  </si>
-  <si>
-    <t>2x treat bowl with cored &amp; scored apple. Inside apple: 1 cranberry and some mlw
-Removed: TE removed at PM check. Both apples had been removed from bowls and pecked at.
-Eval: Extreme interest</t>
-  </si>
-  <si>
-    <t>Placed treat bowl with lettuce, cranberries in house.
-Removed:  CC check, 10 Dec 2019, MW
-Eval: Moderate extreme interest. One bowl had lettuce out of it along with cranberries missing.  Second bowl had 2 cranberries beside bowl, lettuce still in it.</t>
-  </si>
-  <si>
-    <t>2x treat bowl with sweet corn, 4 clem wedges, 3 blueberries covered with leaves.
-Removed: 12/14 in PM by JC
-Eval: found a clem next to bowl and leaves around bowls. corn and blueberries gone, 2 clem gone.</t>
-  </si>
-  <si>
-    <t>2 small treat bowls with lettuce and 3 grapes per bowl.
-Removed: 12/21 in PM by JC
-Eval: grapes gone and most of lettuce gone</t>
-  </si>
-  <si>
-    <t>2x treat bowl with lettuce, corn, pomegranate seeds and carrot chunks
-removed: 12/28 in afternoon 
-Eval: lettuce out of bowl, corn gone, some pom seeds still left.</t>
-  </si>
-  <si>
-    <t>(2) treat bowl with 3 clementine wedges, 5-6 blueberries, and small amount of sweet corn and peas.
-Removed: 12/31 during PM CC check by TE.
-Eval: Extreme interest. All the treats were gone from both of the bowls.</t>
-  </si>
-  <si>
-    <t>(X2) small treat bowls with wood chips, grapes, blueberries, and mealworms. 
-Removed: 1/4 during PM check by TE. 
-Eval: Extreme interest. All the treats were gone and some of the wood chips were pulled out.</t>
-  </si>
-  <si>
-    <t>2x treat bowl with lettuce, mlws and 2 cored peppers
+Eval: Most straw pulled out of bowl, mlws gone, pom seeds left</t>
+  </si>
+  <si>
+    <t>Small treat bowl with some rocks, paper shreds and blueberries placed in house.
+Removed: 1/10 PM JC
+Eval: Bowl flipped, treats gone.</t>
+  </si>
+  <si>
+    <t>Small treat bowl with christmas tree branches, pomegranite seeds, and cranberries placed inside first half of house. 
+Date/time removed: 1/12/20 16:00 AV
+Eval: No interest, looked untouched.</t>
+  </si>
+  <si>
+    <t>Gave small treat bowl with sand, rocks and mealworms.</t>
+  </si>
+  <si>
+    <t>Treat bowl planted with grass, some mealworms and blueberries on top.
+Removed: 16 jan 1600 by KB
+Eval: Grasses torn out; blueberries foud &amp; removed from shavings.</t>
+  </si>
+  <si>
+    <t>small treat bowl with bark chips, 2 grapes, mealworms, and covered with pieces of fir branches.
+Removed: 19 Jan @1600 KB
+Eval: Appeared untouched.</t>
+  </si>
+  <si>
+    <t>Description/ placement: treat bowl with hay, pomegranate seeds, and 2 grapes placed on W side of house
+Removed date/initials: 23 Jan MB
+Evaluation: About half of the hay was pulled out of bowl, all treats left</t>
+  </si>
+  <si>
+    <t>Description/ placement: Treat bowl with evergreen branches, blueberries and corn.  Placed in back half of house in veiw of door. (MW)
+Removed date/initials: 1/30 JC
+Evaluation: untouched</t>
+  </si>
+  <si>
+    <t>Description/ placement: treat bowl with bark chips, blueberries and leaves hidden.
+Removed date/initials: 2 Feb CG
+Evaluation:  No interest; looked untouched.</t>
+  </si>
+  <si>
+    <t>1 small treat bowl with 2 blue gelatin cubes that contained peanuts, dry mealworms, and blueberries. These were covered with oak leaves and floating in a inch or so of water. **Removed in PM by MB, no interest. Everything still in bowl and looked untouched</t>
+  </si>
+  <si>
+    <t>Treat bowl with newspaper strips, some mlws and 3 clementine wedges.
 Removed:
 Eval:</t>
   </si>
   <si>
-    <t>(2) treat bowl with 2 smelt, some cranberries and some sweet corn.
-Removed: p.m. check 14 Jan
-Eval: mild interest  One treat bowl smelt may have been pecked but all cranberries/corn seemed to be there.  2nd treat bowl - 2 cranberries gone smelt, corn left in bowl.</t>
-  </si>
-  <si>
-    <t>2x treat bowl with a cored and scored apple and mlws inside. A few large pieces of lettuce underneath apple
-Removed: 1/18 Pm JC
-Eval: I did not find apple, lettuce everywhere.</t>
-  </si>
-  <si>
-    <t>(2) treat bowls with a half of a small pumpkin in each, mealworms on top, underneath pumpkin is some shredded brown paper.
-Removed by: AV 11/25.  Mealworms eaten and the pumpkins had lots of peck marks in therm. Brown paper pieces had been pulled out of the bowls.</t>
-  </si>
-  <si>
-    <t>(2) small treat bowls with bark chips, and half of a scored red pepper on top. Mealworms were hidden in bark chips and a few inside the cup of the pepper.
-Date removed:  26 Nov
-Eval:  Extreme interest, peppers pecked, everything tossed outside bowls - CG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(2) treat bowl of top soil with a slotted wiffle ball inside with mealworms inside and some slices of green pepper sticking out the slots.
-Removed: 11/27 @ 1500
-Evaluation: no mlws left, both wiffle balls moved around E section, only 1 green pepper left that I saw. Extreme interest. MB
-</t>
-  </si>
-  <si>
-    <t>(2) small treat bowls of bark chips with pomegranate seeds mixed in. Placed in center section of house.
-Removed: 12/2 AV
-Eval: Bark chips scattered all over and all the pomegranate seeds gone.</t>
-  </si>
-  <si>
-    <t>2 treat bowls with head of lettuce inside.  Core of lettuce removed and mealworms placed on top.
-Removed: AV 12/4 15:15pm
-Eval: HIGHLY successful. The lettuce was completely shredded and scattered around the bowls. It took me 10 minutes at least to clean it all up!</t>
-  </si>
-  <si>
-    <t>(2) treat bowl with half a cored apple, scored. mealworms and some leaves over top. *Apple &amp; mlws gone, many leaves scattered out of bowl.*</t>
-  </si>
-  <si>
-    <t>Small treat bowl with half a pumpkin placed in E side of house.
-Removed: 12/11 PM by MB
-Eval: Tons of peck marks in both pumpkins. Extreme interest
-This note added to the following animals: 040016, 040015</t>
-  </si>
-  <si>
-    <t>(2) small treat bowl with half a head of iceberg lettuce, kernels of field corn wedged into it, some mealworms and a couple blueberries beneath.
-Removed:12/16 AV 15:00
-Eval: EXTREME interest. Every leaf of lettuce was pulled apart and strewn around outside the bowls. No other treats remained.</t>
-  </si>
-  <si>
-    <t>2 small treat bowl with two clementine slices,  mealworms, corn, and leaves covering the top  placed inside house on East end.
-Removed: 17 Dec PM
-Eval: Extreme interest; everything outside of the bowl, corn gone, clementines pecked at</t>
-  </si>
-  <si>
-    <t>2 small treat bowls with dirt, mealworms, peanuts with shell covered with straw. Placed on E side of house.
-Removed: 12/18 PM by MB
-Eval: Straw pulled out of bowl, no treats leftover. Extreme interest</t>
-  </si>
-  <si>
-    <t>two small smelt bowls w/ mealworms, clementine wedges, and covered with shredded newspaper. 
-Removed: 23 Dec PM
-Evaluation:  Moderate interest; treats gone, some paper pulled out of bowl.</t>
-  </si>
-  <si>
-    <t>2 treat bowls with mulch, leaves and blueberries. 
-Removed: 
-Eval:</t>
-  </si>
-  <si>
-    <t>2x treat bowls with 2 paper towel roll spheres in each. Inside spheres were some shelled peanuts and pomegranate seeds
-Removed: 1/1 in afternoon JC
-Eval: spheres torn apart, treats gone</t>
-  </si>
-  <si>
-    <t>Enrichment given:  Treat bowls with bark, wiffle ball with ~ a dozen mealworms inside.
-Date/Time removed: 1/6 15:00 AV
-Evaluation: One treat bowl was flipped over, bark chips scattered everywhere and the wiffle balls were out and had no mealworms remaining!</t>
-  </si>
-  <si>
-    <t>This note added to the following animals: 040016, 040015
-Placed 2 bowls w/leaves, sand and clementines in house.
-By PM check, clementines gone.</t>
-  </si>
-  <si>
-    <t>2x treat bowl with bark chips, mlws and some field corn
-Removed: 1/8 during PM CC check.
-Eval: Extreme interest. Some bark chips were pulled out and all the treats were gone.</t>
-  </si>
-  <si>
-    <t>Enrichment given: Treat bowls with leaves, pomagrante chunk
-Date/Time removed: 1/13 AV
-Evaluation: A few pom seeds missing off the chunk, but not many. Leaves were scattered outside bowls.</t>
-  </si>
-  <si>
-    <t>2x treat bowl with sand, river rocks, mlws and dried leaves
+    <t>Small treat bowl with lettuce, blueberries, and an ice cube with misc treats and a bit of water in bowl. Placed in front of house along the divider in West corner.
+Removed: 12/20 PM by MB
+Eval: Bowl completely empty, lettuce and blueberries scattered</t>
+  </si>
+  <si>
+    <t>Treat bowl with water, lettuce, clem wedge and blueberries
+Removed: 12/27 by MB
+Eval: Lettuce scattered out of bowl, water spilled, treats not eaten</t>
+  </si>
+  <si>
+    <t>Small treat bowl of pom seeds, 2 brussel sprouts, thin layer of water covering treats and leaves covering that. **she ran up to bowl but then seemed disapointed**
+Removed: 1/3 PM by MB
+Eval: 1 brussel sprout out of bowl, some water spilled, pom seeds still left</t>
+  </si>
+  <si>
+    <t>MW placed treat bowl with ~1inch of water, evergreen branches, 2 clementine slices and dried mlws in house
+Removed: 17 Jan, KT
+Eval:  For most part looked untouched.  Clementine slices and some mealworms still in bowl.  Removed.</t>
+  </si>
+  <si>
+    <t>Description/ placement: treat bowl with water, 2 cored peppers and some lettuce
+Removed date/initials: 24 Jan, KT
+Evaluation: Lettuce and peppers laying in shavings.  Peppers looked played with but not eaten.</t>
+  </si>
+  <si>
+    <t>Description/ placement: treat bowl with ~1in water, a few small evergreen branches, 2 big but thin apple slices and 2 treat ice cubes. Placed on W side of house
+Removed date/initials: 31 Jan MB
+Evaluation: A few shavings in water so she might've poked around in it but no treats out of bowl or eaten</t>
+  </si>
+  <si>
+    <t>1 small treat bowl with sliced pears, a few clementine slices, and lettuce. Placed in frotn half of house. She went up to it right away and was pushing the items around, but didn't seem to want to eat any of it.**Removed by ZZ ~1645. Lettuce tossed out of bowl, rest left in bowl. Moderate interest**</t>
+  </si>
+  <si>
+    <t>Treat bowl with lettuce, a few peanuts, small squash slices and a pear slice in W side of house. When I checked thru window she was already interacting with it.
+Removed: 30 Nov, KT
+Eval: Everything looked to be played with and peanuts eaten.</t>
+  </si>
+  <si>
+    <t>Small bowl with corn kernels, yellow squash slices, and pomegranate covered with leaves. **2 leaves removed, few if any food items eaten.</t>
+  </si>
+  <si>
+    <t>Cored out apple with mealworms and cranberry in the middle placed inside first half of house. 
+Removed: TE removed at PM check. No treats had been eaten and apple looked untouched besides being on its side instead of remaining upright.
+Evaluation: No interest</t>
+  </si>
+  <si>
+    <t>Small treat bowl with mealworms, cranberries, and lettuce provided inside house. 
+Removed: 10 DEc, 1550
+Eval: *started eating mealworms right away when the bowl was set down*.  3 pieces of lettuce were outside the bowl.  Did find 2 mealworms under lettuce frozen to bottom of bowl.</t>
+  </si>
+  <si>
+    <t>Small treat bowl with lettuce and apple pieces placed inside house.
+Removed: 13 Dec PM, KT
+Eval:  Looked untouched.</t>
+  </si>
+  <si>
+    <t>A treat bowl with sweet corn, 4 clem wedges, 3 blueberries covered with leaves. placed in front side of house.
+Removed: 12/14 in pm by JC
+Eval: corn and blueberries gone. clem wedges out of bowl, a few leaves out of bowl.</t>
+  </si>
+  <si>
+    <t>Small treat bowl with two clementine slices, mealworms, corn, and leaves covering the top placed inside first half of house. 
+Removed by &amp; date: 17 Dec PM
+Eval:  Leaves removed &amp; torn apart &amp; some mealworms gone but other food items left in bowl.</t>
+  </si>
+  <si>
+    <t>1 small treat bowl with lettuce and 3 grapes. Placed in the front of the house.
+Removed: 12/21 in PM by JC
+Eval: everything was untouched. I tossed her a grape to get her in the house, so there may be a grape in the house still in the Am 12/22</t>
+  </si>
+  <si>
+    <t>treat bowl with lettuce, corn, pomegranate seeds and carrot chunks. **left in with her for the day**
+removed: 12/29 am
+Eval: bowl tipped over and most of treats looked untouched</t>
+  </si>
+  <si>
+    <t>carrot and potato chunks, and mealworms in a small treat bowl. A couple inches of water in bowl. Placed in yard outside gate.
+removed: 12/29 PM by MB
+eval: **she was eating the mlws out of bowl as soon as I sat it down, knocked out the other treats** bowl tipped over, mlws gone</t>
+  </si>
+  <si>
+    <t>treat bowl with 3 clementine wedges, 5-6 blueberries, and small amount of sweet corn and peas.
 Removed:
 Eval:</t>
   </si>
   <si>
-    <t>2 paper lunch bags (cut short) with top soil, some seeds and mealworms on top.  3 pieces of newspaper were across the top of the paper bag, fitted into slits.
-Removed: 1/20 AV
-Eval: Untouched</t>
-  </si>
-  <si>
-    <t>Column1</t>
+    <t>treat bowl with bark, mlws, a couple blueberries and a grape
+Removed: 1/4 during PM check by TE.
+Eval: Moderate interest. Some of the bark was pulled out and it appeared like a few blueberries and mealworms were eaten.</t>
+  </si>
+  <si>
+    <t>Small treat bowl with one smelt and pieces of corn placed inside first half of house. 
+Date/time removed: 14 Jan afternoon check
+Eval: mild interest - smelt gone -lots of corn left in bowl</t>
+  </si>
+  <si>
+    <t>TE placed treat bowl with a cored and scored apple and mlws inside. A few large pieces of lettuce underneath apple
+Removed: 1/18 PM JC
+Eval: apple out of bowl, and lettuce out of bowl. mlws gone.</t>
+  </si>
+  <si>
+    <t>Enrichment given:  Treat owls with cranberries &amp; clementine pieces placed inside house. 
+Date/Time removed: 1/21 during PM CC check.
+Evaluation: Extreme interest. Everything was taken out of bowl and spread around.</t>
+  </si>
+  <si>
+    <t>Description/ placement: Treat bowl with dirt, mlws, field corn and some frozen peas
+Removed date/initials: 1/25 JC
+Evaluation: no treats found, dirt everywhere</t>
+  </si>
+  <si>
+    <t>Description/ placement: treat bowl with lettuce, 1 tbsp  of sprouted seeds, and some mlws placed on E side of house
+Removed date/initials:
+Evaluation:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -712,127 +827,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top style="thin">
-          <color auto="1"/>
-        </top>
-        <bottom style="thin">
-          <color auto="1"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{1F9DD78E-50EF-4E86-AE88-D803937E53D5}" name="Table1" displayName="Table1" ref="A1:T61" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:T61" xr:uid="{DDF152D3-B30C-4B75-B9A7-CDAFA4BD7E4F}"/>
-  <tableColumns count="20">
-    <tableColumn id="1" xr3:uid="{D419E60F-82CF-4240-B9EE-19CB1D69A322}" name="Column1" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{83C72ED4-FDBF-4CC3-A07A-1058C1CE68D2}" name="individual"/>
-    <tableColumn id="3" xr3:uid="{6382CDFD-E6B8-496B-AF98-CE7646C541EB}" name="localId"/>
-    <tableColumn id="4" xr3:uid="{F76CBF58-EF9D-4FE2-8DF7-052564870EC1}" name="preferredID"/>
-    <tableColumn id="5" xr3:uid="{C2082587-2F90-4A7D-A06C-5CDB4BBD8382}" name="species"/>
-    <tableColumn id="6" xr3:uid="{C879FC8A-A6F9-4E71-8A90-C7C585A36D1B}" name="birth_loc"/>
-    <tableColumn id="7" xr3:uid="{DE1C1B46-53A9-4E9C-94EE-A8A635BE6851}" name="birth_type"/>
-    <tableColumn id="8" xr3:uid="{81D31227-9457-4EF8-AA7C-49A6BDE41622}" name="birthAge"/>
-    <tableColumn id="9" xr3:uid="{D4642136-9D67-40C1-891A-35A0451EB152}" name="current_collection"/>
-    <tableColumn id="10" xr3:uid="{4B2BDFF6-4BB9-4D01-B81E-D853FFFF97AC}" name="current_enclosure"/>
-    <tableColumn id="11" xr3:uid="{6B6C39DC-B6D0-4206-8D9E-40EDC6DFE466}" name="enrichmentType"/>
-    <tableColumn id="12" xr3:uid="{E4B06B80-B2E1-48C2-A878-89CB25EBDCC2}" name="eCategory"/>
-    <tableColumn id="13" xr3:uid="{B5869F1A-FA03-41C0-A0AB-99861C660AB4}" name="eGoal"/>
-    <tableColumn id="14" xr3:uid="{613AF4B2-C06B-4360-B726-D150E0F08710}" name="eDate"/>
-    <tableColumn id="15" xr3:uid="{4325A931-C565-46C1-B00D-F1B1185E5AB8}" name="dateGiven" dataDxfId="0"/>
-    <tableColumn id="16" xr3:uid="{342F123D-2003-4A96-8FE2-EA06FC6D4039}" name="timeGiven"/>
-    <tableColumn id="17" xr3:uid="{555BECA0-9EDB-486B-9B3E-C2512E41FA73}" name="reaction"/>
-    <tableColumn id="18" xr3:uid="{22E553C6-FA12-40E4-A501-62247784DB83}" name="rating"/>
-    <tableColumn id="19" xr3:uid="{8347EE29-FFCB-4865-B259-975DA79D89EE}" name="providedBy"/>
-    <tableColumn id="20" xr3:uid="{922E7A6D-664F-4417-9BF2-A5B656BA5AFA}" name="details"/>
-  </tableColumns>
-  <tableStyleInfo name="TableStyleLight11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -878,7 +884,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -910,27 +916,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -962,24 +950,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1155,40 +1125,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T61"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:T73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I13" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="55.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="34.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="36.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="32" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.85546875" style="3" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="255.7109375" bestFit="1" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>173</v>
-      </c>
+    <row r="1" spans="1:20">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1228,7 +1172,7 @@
       <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
       <c r="P1" s="1" t="s">
@@ -1247,7 +1191,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1290,20 +1234,26 @@
       <c r="N2" t="s">
         <v>32</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="O2" t="s">
         <v>33</v>
       </c>
+      <c r="P2" t="s">
+        <v>105</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>112</v>
+      </c>
       <c r="R2" t="s">
-        <v>101</v>
+        <v>119</v>
       </c>
       <c r="S2" t="s">
-        <v>104</v>
+        <v>124</v>
       </c>
       <c r="T2" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1346,26 +1296,26 @@
       <c r="N3" t="s">
         <v>32</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="O3" t="s">
         <v>34</v>
       </c>
       <c r="P3" t="s">
-        <v>92</v>
+        <v>106</v>
       </c>
       <c r="Q3" t="s">
-        <v>96</v>
+        <v>113</v>
       </c>
       <c r="R3" t="s">
-        <v>101</v>
+        <v>119</v>
       </c>
       <c r="S3" t="s">
-        <v>105</v>
+        <v>125</v>
       </c>
       <c r="T3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1408,26 +1358,26 @@
       <c r="N4" t="s">
         <v>32</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="O4" t="s">
         <v>35</v>
       </c>
       <c r="P4" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="Q4" t="s">
-        <v>96</v>
+        <v>114</v>
       </c>
       <c r="R4" t="s">
-        <v>101</v>
+        <v>119</v>
       </c>
       <c r="S4" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="T4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1470,26 +1420,26 @@
       <c r="N5" t="s">
         <v>32</v>
       </c>
-      <c r="O5" s="3" t="s">
+      <c r="O5" t="s">
         <v>36</v>
       </c>
       <c r="P5" t="s">
-        <v>93</v>
+        <v>105</v>
       </c>
       <c r="Q5" t="s">
-        <v>97</v>
+        <v>112</v>
       </c>
       <c r="R5" t="s">
-        <v>101</v>
+        <v>120</v>
       </c>
       <c r="S5" t="s">
-        <v>104</v>
+        <v>127</v>
       </c>
       <c r="T5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1532,26 +1482,17 @@
       <c r="N6" t="s">
         <v>32</v>
       </c>
-      <c r="O6" s="3" t="s">
+      <c r="O6" t="s">
         <v>37</v>
       </c>
       <c r="P6" t="s">
-        <v>93</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>98</v>
-      </c>
-      <c r="R6" t="s">
-        <v>102</v>
-      </c>
-      <c r="S6" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="T6" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="7" spans="1:20">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1594,26 +1535,26 @@
       <c r="N7" t="s">
         <v>32</v>
       </c>
-      <c r="O7" s="3" t="s">
+      <c r="O7" t="s">
         <v>38</v>
       </c>
       <c r="P7" t="s">
-        <v>92</v>
+        <v>106</v>
       </c>
       <c r="Q7" t="s">
-        <v>97</v>
+        <v>115</v>
       </c>
       <c r="R7" t="s">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="S7" t="s">
-        <v>105</v>
+        <v>128</v>
       </c>
       <c r="T7" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1656,26 +1597,23 @@
       <c r="N8" t="s">
         <v>32</v>
       </c>
-      <c r="O8" s="3" t="s">
+      <c r="O8" t="s">
         <v>39</v>
       </c>
-      <c r="P8" t="s">
-        <v>94</v>
-      </c>
       <c r="Q8" t="s">
-        <v>99</v>
+        <v>113</v>
       </c>
       <c r="R8" t="s">
-        <v>102</v>
+        <v>119</v>
       </c>
       <c r="S8" t="s">
-        <v>104</v>
+        <v>129</v>
       </c>
       <c r="T8" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="9" spans="1:20">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1718,26 +1656,23 @@
       <c r="N9" t="s">
         <v>32</v>
       </c>
-      <c r="O9" s="3" t="s">
+      <c r="O9" t="s">
         <v>40</v>
       </c>
-      <c r="P9" t="s">
-        <v>94</v>
-      </c>
       <c r="Q9" t="s">
-        <v>97</v>
+        <v>114</v>
       </c>
       <c r="R9" t="s">
-        <v>101</v>
+        <v>120</v>
       </c>
       <c r="S9" t="s">
-        <v>104</v>
+        <v>130</v>
       </c>
       <c r="T9" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="10" spans="1:20">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1780,23 +1715,26 @@
       <c r="N10" t="s">
         <v>32</v>
       </c>
-      <c r="O10" s="3" t="s">
+      <c r="O10" t="s">
         <v>41</v>
       </c>
+      <c r="P10" t="s">
+        <v>106</v>
+      </c>
       <c r="Q10" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="R10" t="s">
-        <v>102</v>
+        <v>121</v>
       </c>
       <c r="S10" t="s">
-        <v>106</v>
+        <v>126</v>
       </c>
       <c r="T10" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1839,26 +1777,23 @@
       <c r="N11" t="s">
         <v>32</v>
       </c>
-      <c r="O11" s="3" t="s">
+      <c r="O11" t="s">
         <v>42</v>
       </c>
-      <c r="P11" t="s">
-        <v>92</v>
-      </c>
       <c r="Q11" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="R11" t="s">
-        <v>101</v>
+        <v>120</v>
       </c>
       <c r="S11" t="s">
-        <v>105</v>
+        <v>124</v>
       </c>
       <c r="T11" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1901,26 +1836,23 @@
       <c r="N12" t="s">
         <v>32</v>
       </c>
-      <c r="O12" s="3" t="s">
+      <c r="O12" t="s">
         <v>43</v>
       </c>
-      <c r="P12" t="s">
-        <v>93</v>
-      </c>
       <c r="Q12" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="R12" t="s">
-        <v>101</v>
+        <v>120</v>
       </c>
       <c r="S12" t="s">
-        <v>105</v>
+        <v>124</v>
       </c>
       <c r="T12" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1963,26 +1895,23 @@
       <c r="N13" t="s">
         <v>32</v>
       </c>
-      <c r="O13" s="3" t="s">
+      <c r="O13" t="s">
         <v>44</v>
       </c>
-      <c r="P13" t="s">
-        <v>93</v>
-      </c>
       <c r="Q13" t="s">
-        <v>97</v>
+        <v>113</v>
       </c>
       <c r="R13" t="s">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="S13" t="s">
-        <v>107</v>
+        <v>129</v>
       </c>
       <c r="T13" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -2025,14 +1954,14 @@
       <c r="N14" t="s">
         <v>32</v>
       </c>
-      <c r="O14" s="3" t="s">
+      <c r="O14" t="s">
         <v>45</v>
       </c>
       <c r="T14" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -2075,26 +2004,26 @@
       <c r="N15" t="s">
         <v>32</v>
       </c>
-      <c r="O15" s="3" t="s">
+      <c r="O15" t="s">
         <v>46</v>
       </c>
       <c r="P15" t="s">
-        <v>92</v>
+        <v>108</v>
       </c>
       <c r="Q15" t="s">
-        <v>97</v>
+        <v>112</v>
       </c>
       <c r="R15" t="s">
-        <v>101</v>
+        <v>120</v>
       </c>
       <c r="S15" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="T15" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -2137,23 +2066,14 @@
       <c r="N16" t="s">
         <v>32</v>
       </c>
-      <c r="O16" s="3" t="s">
+      <c r="O16" t="s">
         <v>47</v>
       </c>
-      <c r="Q16" t="s">
-        <v>96</v>
-      </c>
-      <c r="R16" t="s">
-        <v>101</v>
-      </c>
-      <c r="S16" t="s">
-        <v>108</v>
-      </c>
       <c r="T16" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="17" spans="1:20">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -2196,14 +2116,23 @@
       <c r="N17" t="s">
         <v>32</v>
       </c>
-      <c r="O17" s="3" t="s">
+      <c r="O17" t="s">
         <v>48</v>
       </c>
+      <c r="Q17" t="s">
+        <v>112</v>
+      </c>
+      <c r="R17" t="s">
+        <v>121</v>
+      </c>
+      <c r="S17" t="s">
+        <v>131</v>
+      </c>
       <c r="T17" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -2246,20 +2175,23 @@
       <c r="N18" t="s">
         <v>32</v>
       </c>
-      <c r="O18" s="3" t="s">
+      <c r="O18" t="s">
         <v>49</v>
       </c>
       <c r="Q18" t="s">
-        <v>96</v>
+        <v>113</v>
       </c>
       <c r="R18" t="s">
-        <v>101</v>
+        <v>119</v>
+      </c>
+      <c r="S18" t="s">
+        <v>129</v>
       </c>
       <c r="T18" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="19" spans="1:20">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -2302,14 +2234,17 @@
       <c r="N19" t="s">
         <v>32</v>
       </c>
-      <c r="O19" s="3" t="s">
+      <c r="O19" t="s">
         <v>50</v>
       </c>
+      <c r="P19" t="s">
+        <v>109</v>
+      </c>
       <c r="T19" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -2352,14 +2287,23 @@
       <c r="N20" t="s">
         <v>32</v>
       </c>
-      <c r="O20" s="3" t="s">
-        <v>50</v>
+      <c r="O20" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>112</v>
+      </c>
+      <c r="R20" t="s">
+        <v>122</v>
+      </c>
+      <c r="S20" t="s">
+        <v>129</v>
       </c>
       <c r="T20" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="21" spans="1:20">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -2402,141 +2346,132 @@
       <c r="N21" t="s">
         <v>32</v>
       </c>
-      <c r="O21" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="P21" t="s">
-        <v>92</v>
+      <c r="O21" t="s">
+        <v>52</v>
       </c>
       <c r="Q21" t="s">
-        <v>97</v>
+        <v>112</v>
       </c>
       <c r="R21" t="s">
-        <v>101</v>
+        <v>120</v>
       </c>
       <c r="S21" t="s">
-        <v>105</v>
+        <v>126</v>
       </c>
       <c r="T21" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" t="s">
+        <v>20</v>
+      </c>
+      <c r="D22" t="s">
+        <v>21</v>
+      </c>
+      <c r="E22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F22" t="s">
+        <v>23</v>
+      </c>
+      <c r="G22" t="s">
+        <v>24</v>
+      </c>
+      <c r="H22" t="s">
+        <v>25</v>
+      </c>
+      <c r="I22" t="s">
+        <v>26</v>
+      </c>
+      <c r="J22" t="s">
+        <v>27</v>
+      </c>
+      <c r="K22" t="s">
+        <v>28</v>
+      </c>
+      <c r="L22" t="s">
+        <v>32</v>
+      </c>
+      <c r="M22" t="s">
+        <v>32</v>
+      </c>
+      <c r="N22" t="s">
+        <v>32</v>
+      </c>
+      <c r="O22" t="s">
+        <v>53</v>
+      </c>
+      <c r="T22" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" t="s">
+        <v>20</v>
+      </c>
+      <c r="D23" t="s">
+        <v>21</v>
+      </c>
+      <c r="E23" t="s">
+        <v>22</v>
+      </c>
+      <c r="F23" t="s">
+        <v>23</v>
+      </c>
+      <c r="G23" t="s">
+        <v>24</v>
+      </c>
+      <c r="H23" t="s">
+        <v>25</v>
+      </c>
+      <c r="I23" t="s">
+        <v>26</v>
+      </c>
+      <c r="J23" t="s">
+        <v>27</v>
+      </c>
+      <c r="K23" t="s">
+        <v>28</v>
+      </c>
+      <c r="L23" t="s">
+        <v>32</v>
+      </c>
+      <c r="M23" t="s">
+        <v>32</v>
+      </c>
+      <c r="N23" t="s">
+        <v>32</v>
+      </c>
+      <c r="O23" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>112</v>
+      </c>
+      <c r="R23" t="s">
+        <v>123</v>
+      </c>
+      <c r="S23" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>20</v>
-      </c>
-      <c r="B22" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" t="s">
-        <v>20</v>
-      </c>
-      <c r="D22" t="s">
-        <v>21</v>
-      </c>
-      <c r="E22" t="s">
-        <v>22</v>
-      </c>
-      <c r="F22" t="s">
-        <v>23</v>
-      </c>
-      <c r="G22" t="s">
-        <v>24</v>
-      </c>
-      <c r="H22" t="s">
-        <v>25</v>
-      </c>
-      <c r="I22" t="s">
-        <v>26</v>
-      </c>
-      <c r="J22" t="s">
-        <v>27</v>
-      </c>
-      <c r="K22" t="s">
-        <v>29</v>
-      </c>
-      <c r="L22" t="s">
-        <v>32</v>
-      </c>
-      <c r="M22" t="s">
-        <v>32</v>
-      </c>
-      <c r="N22" t="s">
-        <v>32</v>
-      </c>
-      <c r="O22" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="P22" t="s">
-        <v>94</v>
-      </c>
-      <c r="T22" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>21</v>
-      </c>
-      <c r="B23" t="s">
-        <v>19</v>
-      </c>
-      <c r="C23" t="s">
-        <v>20</v>
-      </c>
-      <c r="D23" t="s">
-        <v>21</v>
-      </c>
-      <c r="E23" t="s">
-        <v>22</v>
-      </c>
-      <c r="F23" t="s">
-        <v>23</v>
-      </c>
-      <c r="G23" t="s">
-        <v>24</v>
-      </c>
-      <c r="H23" t="s">
-        <v>25</v>
-      </c>
-      <c r="I23" t="s">
-        <v>26</v>
-      </c>
-      <c r="J23" t="s">
-        <v>27</v>
-      </c>
-      <c r="K23" t="s">
-        <v>29</v>
-      </c>
-      <c r="L23" t="s">
-        <v>32</v>
-      </c>
-      <c r="M23" t="s">
-        <v>32</v>
-      </c>
-      <c r="N23" t="s">
-        <v>32</v>
-      </c>
-      <c r="O23" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="P23" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q23" t="s">
-        <v>99</v>
-      </c>
-      <c r="R23" t="s">
-        <v>101</v>
-      </c>
-      <c r="S23" t="s">
-        <v>104</v>
-      </c>
       <c r="T23" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -2568,7 +2503,7 @@
         <v>27</v>
       </c>
       <c r="K24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L24" t="s">
         <v>32</v>
@@ -2579,26 +2514,20 @@
       <c r="N24" t="s">
         <v>32</v>
       </c>
-      <c r="O24" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="P24" t="s">
-        <v>93</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>100</v>
+      <c r="O24" t="s">
+        <v>55</v>
       </c>
       <c r="R24" t="s">
-        <v>102</v>
+        <v>120</v>
       </c>
       <c r="S24" t="s">
-        <v>104</v>
+        <v>126</v>
       </c>
       <c r="T24" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -2630,7 +2559,7 @@
         <v>27</v>
       </c>
       <c r="K25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L25" t="s">
         <v>32</v>
@@ -2641,17 +2570,20 @@
       <c r="N25" t="s">
         <v>32</v>
       </c>
-      <c r="O25" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="P25" t="s">
-        <v>92</v>
+      <c r="O25" t="s">
+        <v>56</v>
+      </c>
+      <c r="R25" t="s">
+        <v>119</v>
+      </c>
+      <c r="S25" t="s">
+        <v>124</v>
       </c>
       <c r="T25" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -2683,7 +2615,7 @@
         <v>27</v>
       </c>
       <c r="K26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L26" t="s">
         <v>32</v>
@@ -2694,23 +2626,20 @@
       <c r="N26" t="s">
         <v>32</v>
       </c>
-      <c r="O26" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="Q26" t="s">
-        <v>96</v>
+      <c r="O26" t="s">
+        <v>57</v>
       </c>
       <c r="R26" t="s">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="S26" t="s">
-        <v>104</v>
+        <v>126</v>
       </c>
       <c r="T26" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -2742,7 +2671,7 @@
         <v>27</v>
       </c>
       <c r="K27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="L27" t="s">
         <v>32</v>
@@ -2753,23 +2682,14 @@
       <c r="N27" t="s">
         <v>32</v>
       </c>
-      <c r="O27" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>96</v>
-      </c>
-      <c r="R27" t="s">
-        <v>101</v>
-      </c>
-      <c r="S27" t="s">
-        <v>104</v>
+      <c r="O27" t="s">
+        <v>58</v>
       </c>
       <c r="T27" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -2812,23 +2732,26 @@
       <c r="N28" t="s">
         <v>32</v>
       </c>
-      <c r="O28" s="3" t="s">
-        <v>58</v>
+      <c r="O28" t="s">
+        <v>59</v>
+      </c>
+      <c r="P28" t="s">
+        <v>110</v>
       </c>
       <c r="Q28" t="s">
-        <v>98</v>
+        <v>114</v>
       </c>
       <c r="R28" t="s">
-        <v>102</v>
+        <v>120</v>
       </c>
       <c r="S28" t="s">
-        <v>104</v>
+        <v>126</v>
       </c>
       <c r="T28" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -2871,23 +2794,26 @@
       <c r="N29" t="s">
         <v>32</v>
       </c>
-      <c r="O29" s="3" t="s">
-        <v>59</v>
+      <c r="O29" t="s">
+        <v>60</v>
+      </c>
+      <c r="P29" t="s">
+        <v>106</v>
       </c>
       <c r="Q29" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="R29" t="s">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="S29" t="s">
-        <v>104</v>
+        <v>131</v>
       </c>
       <c r="T29" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -2919,7 +2845,7 @@
         <v>27</v>
       </c>
       <c r="K30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L30" t="s">
         <v>32</v>
@@ -2930,14 +2856,26 @@
       <c r="N30" t="s">
         <v>32</v>
       </c>
-      <c r="O30" s="3" t="s">
-        <v>60</v>
+      <c r="O30" t="s">
+        <v>61</v>
+      </c>
+      <c r="P30" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>116</v>
+      </c>
+      <c r="R30" t="s">
+        <v>120</v>
+      </c>
+      <c r="S30" t="s">
+        <v>133</v>
       </c>
       <c r="T30" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -2969,7 +2907,7 @@
         <v>27</v>
       </c>
       <c r="K31" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L31" t="s">
         <v>32</v>
@@ -2980,17 +2918,26 @@
       <c r="N31" t="s">
         <v>32</v>
       </c>
-      <c r="O31" s="3" t="s">
-        <v>61</v>
+      <c r="O31" t="s">
+        <v>62</v>
       </c>
       <c r="P31" t="s">
-        <v>93</v>
+        <v>106</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>114</v>
+      </c>
+      <c r="R31" t="s">
+        <v>120</v>
+      </c>
+      <c r="S31" t="s">
+        <v>126</v>
       </c>
       <c r="T31" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -3022,7 +2969,7 @@
         <v>27</v>
       </c>
       <c r="K32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L32" t="s">
         <v>32</v>
@@ -3033,23 +2980,26 @@
       <c r="N32" t="s">
         <v>32</v>
       </c>
-      <c r="O32" s="3" t="s">
-        <v>62</v>
+      <c r="O32" t="s">
+        <v>63</v>
       </c>
       <c r="P32" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="Q32" t="s">
-        <v>97</v>
+        <v>112</v>
       </c>
       <c r="R32" t="s">
-        <v>101</v>
+        <v>120</v>
+      </c>
+      <c r="S32" t="s">
+        <v>132</v>
       </c>
       <c r="T32" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -3081,7 +3031,7 @@
         <v>27</v>
       </c>
       <c r="K33" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L33" t="s">
         <v>32</v>
@@ -3092,26 +3042,26 @@
       <c r="N33" t="s">
         <v>32</v>
       </c>
-      <c r="O33" s="3" t="s">
-        <v>63</v>
+      <c r="O33" t="s">
+        <v>64</v>
       </c>
       <c r="P33" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="Q33" t="s">
-        <v>96</v>
+        <v>114</v>
       </c>
       <c r="R33" t="s">
-        <v>101</v>
+        <v>120</v>
       </c>
       <c r="S33" t="s">
-        <v>104</v>
+        <v>129</v>
       </c>
       <c r="T33" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -3143,7 +3093,7 @@
         <v>27</v>
       </c>
       <c r="K34" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L34" t="s">
         <v>32</v>
@@ -3154,20 +3104,20 @@
       <c r="N34" t="s">
         <v>32</v>
       </c>
-      <c r="O34" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="P34" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q34" t="s">
-        <v>97</v>
+      <c r="O34" t="s">
+        <v>65</v>
+      </c>
+      <c r="R34" t="s">
+        <v>120</v>
+      </c>
+      <c r="S34" t="s">
+        <v>124</v>
       </c>
       <c r="T34" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -3199,7 +3149,7 @@
         <v>27</v>
       </c>
       <c r="K35" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L35" t="s">
         <v>32</v>
@@ -3210,26 +3160,23 @@
       <c r="N35" t="s">
         <v>32</v>
       </c>
-      <c r="O35" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="P35" t="s">
-        <v>93</v>
+      <c r="O35" t="s">
+        <v>66</v>
       </c>
       <c r="Q35" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
       <c r="R35" t="s">
-        <v>102</v>
+        <v>119</v>
       </c>
       <c r="S35" t="s">
-        <v>104</v>
+        <v>129</v>
       </c>
       <c r="T35" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -3261,7 +3208,7 @@
         <v>27</v>
       </c>
       <c r="K36" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L36" t="s">
         <v>32</v>
@@ -3272,17 +3219,23 @@
       <c r="N36" t="s">
         <v>32</v>
       </c>
-      <c r="O36" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="P36" t="s">
-        <v>92</v>
+      <c r="O36" t="s">
+        <v>67</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>112</v>
+      </c>
+      <c r="R36" t="s">
+        <v>121</v>
+      </c>
+      <c r="S36" t="s">
+        <v>132</v>
       </c>
       <c r="T36" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="37" spans="1:20">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -3314,7 +3267,7 @@
         <v>27</v>
       </c>
       <c r="K37" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L37" t="s">
         <v>32</v>
@@ -3325,14 +3278,20 @@
       <c r="N37" t="s">
         <v>32</v>
       </c>
-      <c r="O37" s="3" t="s">
-        <v>67</v>
+      <c r="O37" t="s">
+        <v>68</v>
+      </c>
+      <c r="P37" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>112</v>
       </c>
       <c r="T37" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -3364,7 +3323,7 @@
         <v>27</v>
       </c>
       <c r="K38" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L38" t="s">
         <v>32</v>
@@ -3375,26 +3334,23 @@
       <c r="N38" t="s">
         <v>32</v>
       </c>
-      <c r="O38" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="P38" t="s">
-        <v>93</v>
+      <c r="O38" t="s">
+        <v>69</v>
       </c>
       <c r="Q38" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="R38" t="s">
-        <v>101</v>
+        <v>122</v>
       </c>
       <c r="S38" t="s">
-        <v>105</v>
+        <v>124</v>
       </c>
       <c r="T38" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -3426,7 +3382,7 @@
         <v>27</v>
       </c>
       <c r="K39" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L39" t="s">
         <v>32</v>
@@ -3437,23 +3393,23 @@
       <c r="N39" t="s">
         <v>32</v>
       </c>
-      <c r="O39" s="3" t="s">
-        <v>69</v>
+      <c r="O39" t="s">
+        <v>70</v>
       </c>
       <c r="Q39" t="s">
-        <v>96</v>
+        <v>113</v>
       </c>
       <c r="R39" t="s">
-        <v>101</v>
+        <v>119</v>
       </c>
       <c r="S39" t="s">
-        <v>107</v>
+        <v>134</v>
       </c>
       <c r="T39" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -3485,7 +3441,7 @@
         <v>27</v>
       </c>
       <c r="K40" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L40" t="s">
         <v>32</v>
@@ -3496,14 +3452,14 @@
       <c r="N40" t="s">
         <v>32</v>
       </c>
-      <c r="O40" s="3" t="s">
-        <v>70</v>
+      <c r="O40" t="s">
+        <v>71</v>
       </c>
       <c r="T40" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -3535,7 +3491,7 @@
         <v>27</v>
       </c>
       <c r="K41" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L41" t="s">
         <v>32</v>
@@ -3546,26 +3502,23 @@
       <c r="N41" t="s">
         <v>32</v>
       </c>
-      <c r="O41" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="P41" t="s">
-        <v>94</v>
+      <c r="O41" t="s">
+        <v>72</v>
       </c>
       <c r="Q41" t="s">
-        <v>97</v>
+        <v>112</v>
       </c>
       <c r="R41" t="s">
-        <v>102</v>
+        <v>122</v>
       </c>
       <c r="S41" t="s">
-        <v>105</v>
+        <v>129</v>
       </c>
       <c r="T41" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -3597,7 +3550,7 @@
         <v>27</v>
       </c>
       <c r="K42" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="L42" t="s">
         <v>32</v>
@@ -3608,14 +3561,14 @@
       <c r="N42" t="s">
         <v>32</v>
       </c>
-      <c r="O42" s="3" t="s">
-        <v>72</v>
+      <c r="O42" t="s">
+        <v>73</v>
       </c>
       <c r="T42" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -3647,7 +3600,7 @@
         <v>27</v>
       </c>
       <c r="K43" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="L43" t="s">
         <v>32</v>
@@ -3658,26 +3611,14 @@
       <c r="N43" t="s">
         <v>32</v>
       </c>
-      <c r="O43" s="3" t="s">
-        <v>73</v>
-      </c>
-      <c r="P43" t="s">
-        <v>93</v>
-      </c>
-      <c r="Q43" t="s">
-        <v>99</v>
-      </c>
-      <c r="R43" t="s">
-        <v>101</v>
-      </c>
-      <c r="S43" t="s">
-        <v>105</v>
+      <c r="O43" t="s">
+        <v>74</v>
       </c>
       <c r="T43" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -3709,7 +3650,7 @@
         <v>27</v>
       </c>
       <c r="K44" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="L44" t="s">
         <v>32</v>
@@ -3720,26 +3661,14 @@
       <c r="N44" t="s">
         <v>32</v>
       </c>
-      <c r="O44" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="P44" t="s">
-        <v>94</v>
-      </c>
-      <c r="Q44" t="s">
-        <v>96</v>
-      </c>
-      <c r="R44" t="s">
-        <v>101</v>
-      </c>
-      <c r="S44" t="s">
-        <v>109</v>
+      <c r="O44" t="s">
+        <v>75</v>
       </c>
       <c r="T44" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -3771,7 +3700,7 @@
         <v>27</v>
       </c>
       <c r="K45" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="L45" t="s">
         <v>32</v>
@@ -3782,26 +3711,20 @@
       <c r="N45" t="s">
         <v>32</v>
       </c>
-      <c r="O45" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="P45" t="s">
-        <v>92</v>
-      </c>
-      <c r="Q45" t="s">
-        <v>96</v>
+      <c r="O45" t="s">
+        <v>76</v>
       </c>
       <c r="R45" t="s">
-        <v>101</v>
+        <v>119</v>
       </c>
       <c r="S45" t="s">
-        <v>105</v>
+        <v>132</v>
       </c>
       <c r="T45" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -3833,7 +3756,7 @@
         <v>27</v>
       </c>
       <c r="K46" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="L46" t="s">
         <v>32</v>
@@ -3844,26 +3767,17 @@
       <c r="N46" t="s">
         <v>32</v>
       </c>
-      <c r="O46" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="P46" t="s">
-        <v>92</v>
-      </c>
-      <c r="Q46" t="s">
-        <v>97</v>
+      <c r="O46" t="s">
+        <v>77</v>
       </c>
       <c r="R46" t="s">
-        <v>101</v>
-      </c>
-      <c r="S46" t="s">
-        <v>105</v>
+        <v>121</v>
       </c>
       <c r="T46" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -3895,7 +3809,7 @@
         <v>27</v>
       </c>
       <c r="K47" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="L47" t="s">
         <v>32</v>
@@ -3906,26 +3820,20 @@
       <c r="N47" t="s">
         <v>32</v>
       </c>
-      <c r="O47" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="P47" t="s">
-        <v>92</v>
-      </c>
-      <c r="Q47" t="s">
-        <v>97</v>
+      <c r="O47" t="s">
+        <v>78</v>
       </c>
       <c r="R47" t="s">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="S47" t="s">
-        <v>110</v>
+        <v>126</v>
       </c>
       <c r="T47" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -3957,7 +3865,7 @@
         <v>27</v>
       </c>
       <c r="K48" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L48" t="s">
         <v>32</v>
@@ -3968,26 +3876,26 @@
       <c r="N48" t="s">
         <v>32</v>
       </c>
-      <c r="O48" s="3" t="s">
-        <v>78</v>
+      <c r="O48" t="s">
+        <v>79</v>
       </c>
       <c r="P48" t="s">
-        <v>92</v>
+        <v>106</v>
       </c>
       <c r="Q48" t="s">
-        <v>99</v>
+        <v>118</v>
       </c>
       <c r="R48" t="s">
-        <v>101</v>
+        <v>121</v>
       </c>
       <c r="S48" t="s">
-        <v>105</v>
+        <v>133</v>
       </c>
       <c r="T48" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -4019,7 +3927,7 @@
         <v>27</v>
       </c>
       <c r="K49" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L49" t="s">
         <v>32</v>
@@ -4030,26 +3938,17 @@
       <c r="N49" t="s">
         <v>32</v>
       </c>
-      <c r="O49" s="3" t="s">
-        <v>79</v>
+      <c r="O49" t="s">
+        <v>80</v>
       </c>
       <c r="P49" t="s">
-        <v>93</v>
-      </c>
-      <c r="Q49" t="s">
-        <v>96</v>
-      </c>
-      <c r="R49" t="s">
-        <v>101</v>
-      </c>
-      <c r="S49" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="T49" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -4081,7 +3980,7 @@
         <v>27</v>
       </c>
       <c r="K50" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L50" t="s">
         <v>32</v>
@@ -4092,26 +3991,26 @@
       <c r="N50" t="s">
         <v>32</v>
       </c>
-      <c r="O50" s="3" t="s">
-        <v>80</v>
+      <c r="O50" t="s">
+        <v>81</v>
       </c>
       <c r="P50" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="Q50" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="R50" t="s">
-        <v>101</v>
+        <v>120</v>
       </c>
       <c r="S50" t="s">
-        <v>105</v>
+        <v>133</v>
       </c>
       <c r="T50" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -4143,7 +4042,7 @@
         <v>27</v>
       </c>
       <c r="K51" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L51" t="s">
         <v>32</v>
@@ -4154,23 +4053,23 @@
       <c r="N51" t="s">
         <v>32</v>
       </c>
-      <c r="O51" s="3" t="s">
-        <v>81</v>
+      <c r="O51" t="s">
+        <v>82</v>
       </c>
       <c r="Q51" t="s">
-        <v>96</v>
+        <v>116</v>
       </c>
       <c r="R51" t="s">
-        <v>101</v>
+        <v>119</v>
       </c>
       <c r="S51" t="s">
-        <v>110</v>
+        <v>135</v>
       </c>
       <c r="T51" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -4202,7 +4101,7 @@
         <v>27</v>
       </c>
       <c r="K52" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L52" t="s">
         <v>32</v>
@@ -4213,26 +4112,26 @@
       <c r="N52" t="s">
         <v>32</v>
       </c>
-      <c r="O52" s="3" t="s">
-        <v>82</v>
+      <c r="O52" t="s">
+        <v>83</v>
       </c>
       <c r="P52" t="s">
-        <v>94</v>
+        <v>106</v>
       </c>
       <c r="Q52" t="s">
-        <v>96</v>
+        <v>113</v>
       </c>
       <c r="R52" t="s">
-        <v>101</v>
+        <v>119</v>
       </c>
       <c r="S52" t="s">
-        <v>111</v>
+        <v>133</v>
       </c>
       <c r="T52" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -4264,7 +4163,7 @@
         <v>27</v>
       </c>
       <c r="K53" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L53" t="s">
         <v>32</v>
@@ -4275,23 +4174,23 @@
       <c r="N53" t="s">
         <v>32</v>
       </c>
-      <c r="O53" s="3" t="s">
-        <v>83</v>
+      <c r="O53" t="s">
+        <v>84</v>
       </c>
       <c r="Q53" t="s">
-        <v>96</v>
+        <v>112</v>
       </c>
       <c r="R53" t="s">
-        <v>102</v>
+        <v>121</v>
       </c>
       <c r="S53" t="s">
-        <v>112</v>
+        <v>132</v>
       </c>
       <c r="T53" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="54" spans="1:20">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -4323,7 +4222,7 @@
         <v>27</v>
       </c>
       <c r="K54" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L54" t="s">
         <v>32</v>
@@ -4334,14 +4233,20 @@
       <c r="N54" t="s">
         <v>32</v>
       </c>
-      <c r="O54" s="3" t="s">
-        <v>84</v>
+      <c r="O54" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q54" t="s">
+        <v>112</v>
+      </c>
+      <c r="R54" t="s">
+        <v>119</v>
       </c>
       <c r="T54" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="55" spans="1:20">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -4373,7 +4278,7 @@
         <v>27</v>
       </c>
       <c r="K55" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L55" t="s">
         <v>32</v>
@@ -4384,14 +4289,20 @@
       <c r="N55" t="s">
         <v>32</v>
       </c>
-      <c r="O55" s="3" t="s">
-        <v>85</v>
+      <c r="O55" t="s">
+        <v>86</v>
+      </c>
+      <c r="R55" t="s">
+        <v>121</v>
+      </c>
+      <c r="S55" t="s">
+        <v>132</v>
       </c>
       <c r="T55" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="56" spans="1:20">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -4434,23 +4345,17 @@
       <c r="N56" t="s">
         <v>32</v>
       </c>
-      <c r="O56" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="Q56" t="s">
-        <v>97</v>
-      </c>
-      <c r="R56" t="s">
-        <v>101</v>
-      </c>
-      <c r="S56" t="s">
-        <v>106</v>
+      <c r="O56" t="s">
+        <v>87</v>
+      </c>
+      <c r="P56" t="s">
+        <v>107</v>
       </c>
       <c r="T56" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="57" spans="1:20">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -4493,23 +4398,23 @@
       <c r="N57" t="s">
         <v>32</v>
       </c>
-      <c r="O57" s="3" t="s">
-        <v>87</v>
+      <c r="O57" t="s">
+        <v>88</v>
+      </c>
+      <c r="P57" t="s">
+        <v>109</v>
       </c>
       <c r="Q57" t="s">
-        <v>97</v>
+        <v>114</v>
       </c>
       <c r="R57" t="s">
-        <v>102</v>
-      </c>
-      <c r="S57" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
       <c r="T57" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="58" spans="1:20">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -4552,26 +4457,26 @@
       <c r="N58" t="s">
         <v>32</v>
       </c>
-      <c r="O58" s="3" t="s">
-        <v>88</v>
+      <c r="O58" t="s">
+        <v>89</v>
       </c>
       <c r="P58" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="Q58" t="s">
-        <v>96</v>
+        <v>115</v>
       </c>
       <c r="R58" t="s">
-        <v>101</v>
+        <v>119</v>
       </c>
       <c r="S58" t="s">
-        <v>104</v>
+        <v>128</v>
       </c>
       <c r="T58" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="59" spans="1:20">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -4614,23 +4519,23 @@
       <c r="N59" t="s">
         <v>32</v>
       </c>
-      <c r="O59" s="3" t="s">
-        <v>89</v>
+      <c r="O59" t="s">
+        <v>90</v>
       </c>
       <c r="Q59" t="s">
-        <v>97</v>
+        <v>117</v>
       </c>
       <c r="R59" t="s">
-        <v>102</v>
+        <v>121</v>
       </c>
       <c r="S59" t="s">
-        <v>106</v>
+        <v>129</v>
       </c>
       <c r="T59" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="60" spans="1:20">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -4673,14 +4578,23 @@
       <c r="N60" t="s">
         <v>32</v>
       </c>
-      <c r="O60" s="3" t="s">
-        <v>90</v>
+      <c r="O60" t="s">
+        <v>91</v>
+      </c>
+      <c r="Q60" t="s">
+        <v>112</v>
+      </c>
+      <c r="R60" t="s">
+        <v>119</v>
+      </c>
+      <c r="S60" t="s">
+        <v>129</v>
       </c>
       <c r="T60" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="61" spans="1:20">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -4723,41 +4637,695 @@
       <c r="N61" t="s">
         <v>32</v>
       </c>
-      <c r="O61" s="3" t="s">
-        <v>91</v>
+      <c r="O61" t="s">
+        <v>92</v>
       </c>
       <c r="Q61" t="s">
+        <v>112</v>
+      </c>
+      <c r="R61" t="s">
+        <v>121</v>
+      </c>
+      <c r="S61" t="s">
+        <v>131</v>
+      </c>
+      <c r="T61" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="62" spans="1:20">
+      <c r="A62" s="1">
+        <v>60</v>
+      </c>
+      <c r="B62" t="s">
+        <v>19</v>
+      </c>
+      <c r="C62" t="s">
+        <v>20</v>
+      </c>
+      <c r="D62" t="s">
+        <v>21</v>
+      </c>
+      <c r="E62" t="s">
+        <v>22</v>
+      </c>
+      <c r="F62" t="s">
+        <v>23</v>
+      </c>
+      <c r="G62" t="s">
+        <v>24</v>
+      </c>
+      <c r="H62" t="s">
+        <v>25</v>
+      </c>
+      <c r="I62" t="s">
+        <v>26</v>
+      </c>
+      <c r="J62" t="s">
+        <v>27</v>
+      </c>
+      <c r="K62" t="s">
+        <v>31</v>
+      </c>
+      <c r="L62" t="s">
+        <v>32</v>
+      </c>
+      <c r="M62" t="s">
+        <v>32</v>
+      </c>
+      <c r="N62" t="s">
+        <v>32</v>
+      </c>
+      <c r="O62" t="s">
+        <v>93</v>
+      </c>
+      <c r="P62" t="s">
+        <v>107</v>
+      </c>
+      <c r="Q62" t="s">
+        <v>115</v>
+      </c>
+      <c r="R62" t="s">
+        <v>119</v>
+      </c>
+      <c r="S62" t="s">
+        <v>133</v>
+      </c>
+      <c r="T62" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="63" spans="1:20">
+      <c r="A63" s="1">
+        <v>61</v>
+      </c>
+      <c r="B63" t="s">
+        <v>19</v>
+      </c>
+      <c r="C63" t="s">
+        <v>20</v>
+      </c>
+      <c r="D63" t="s">
+        <v>21</v>
+      </c>
+      <c r="E63" t="s">
+        <v>22</v>
+      </c>
+      <c r="F63" t="s">
+        <v>23</v>
+      </c>
+      <c r="G63" t="s">
+        <v>24</v>
+      </c>
+      <c r="H63" t="s">
+        <v>25</v>
+      </c>
+      <c r="I63" t="s">
+        <v>26</v>
+      </c>
+      <c r="J63" t="s">
+        <v>27</v>
+      </c>
+      <c r="K63" t="s">
+        <v>31</v>
+      </c>
+      <c r="L63" t="s">
+        <v>32</v>
+      </c>
+      <c r="M63" t="s">
+        <v>32</v>
+      </c>
+      <c r="N63" t="s">
+        <v>32</v>
+      </c>
+      <c r="O63" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q63" t="s">
+        <v>113</v>
+      </c>
+      <c r="R63" t="s">
+        <v>119</v>
+      </c>
+      <c r="S63" t="s">
+        <v>129</v>
+      </c>
+      <c r="T63" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="64" spans="1:20">
+      <c r="A64" s="1">
+        <v>62</v>
+      </c>
+      <c r="B64" t="s">
+        <v>19</v>
+      </c>
+      <c r="C64" t="s">
+        <v>20</v>
+      </c>
+      <c r="D64" t="s">
+        <v>21</v>
+      </c>
+      <c r="E64" t="s">
+        <v>22</v>
+      </c>
+      <c r="F64" t="s">
+        <v>23</v>
+      </c>
+      <c r="G64" t="s">
+        <v>24</v>
+      </c>
+      <c r="H64" t="s">
+        <v>25</v>
+      </c>
+      <c r="I64" t="s">
+        <v>26</v>
+      </c>
+      <c r="J64" t="s">
+        <v>27</v>
+      </c>
+      <c r="K64" t="s">
+        <v>31</v>
+      </c>
+      <c r="L64" t="s">
+        <v>32</v>
+      </c>
+      <c r="M64" t="s">
+        <v>32</v>
+      </c>
+      <c r="N64" t="s">
+        <v>32</v>
+      </c>
+      <c r="O64" t="s">
+        <v>95</v>
+      </c>
+      <c r="P64" t="s">
+        <v>111</v>
+      </c>
+      <c r="T64" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="65" spans="1:20">
+      <c r="A65" s="1">
+        <v>63</v>
+      </c>
+      <c r="B65" t="s">
+        <v>19</v>
+      </c>
+      <c r="C65" t="s">
+        <v>20</v>
+      </c>
+      <c r="D65" t="s">
+        <v>21</v>
+      </c>
+      <c r="E65" t="s">
+        <v>22</v>
+      </c>
+      <c r="F65" t="s">
+        <v>23</v>
+      </c>
+      <c r="G65" t="s">
+        <v>24</v>
+      </c>
+      <c r="H65" t="s">
+        <v>25</v>
+      </c>
+      <c r="I65" t="s">
+        <v>26</v>
+      </c>
+      <c r="J65" t="s">
+        <v>27</v>
+      </c>
+      <c r="K65" t="s">
+        <v>31</v>
+      </c>
+      <c r="L65" t="s">
+        <v>32</v>
+      </c>
+      <c r="M65" t="s">
+        <v>32</v>
+      </c>
+      <c r="N65" t="s">
+        <v>32</v>
+      </c>
+      <c r="O65" t="s">
+        <v>96</v>
+      </c>
+      <c r="P65" t="s">
+        <v>105</v>
+      </c>
+      <c r="T65" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="66" spans="1:20">
+      <c r="A66" s="1">
+        <v>64</v>
+      </c>
+      <c r="B66" t="s">
+        <v>19</v>
+      </c>
+      <c r="C66" t="s">
+        <v>20</v>
+      </c>
+      <c r="D66" t="s">
+        <v>21</v>
+      </c>
+      <c r="E66" t="s">
+        <v>22</v>
+      </c>
+      <c r="F66" t="s">
+        <v>23</v>
+      </c>
+      <c r="G66" t="s">
+        <v>24</v>
+      </c>
+      <c r="H66" t="s">
+        <v>25</v>
+      </c>
+      <c r="I66" t="s">
+        <v>26</v>
+      </c>
+      <c r="J66" t="s">
+        <v>27</v>
+      </c>
+      <c r="K66" t="s">
+        <v>31</v>
+      </c>
+      <c r="L66" t="s">
+        <v>32</v>
+      </c>
+      <c r="M66" t="s">
+        <v>32</v>
+      </c>
+      <c r="N66" t="s">
+        <v>32</v>
+      </c>
+      <c r="O66" t="s">
         <v>97</v>
       </c>
-      <c r="R61" t="s">
+      <c r="P66" t="s">
+        <v>111</v>
+      </c>
+      <c r="R66" t="s">
+        <v>120</v>
+      </c>
+      <c r="S66" t="s">
+        <v>133</v>
+      </c>
+      <c r="T66" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="67" spans="1:20">
+      <c r="A67" s="1">
+        <v>65</v>
+      </c>
+      <c r="B67" t="s">
+        <v>19</v>
+      </c>
+      <c r="C67" t="s">
+        <v>20</v>
+      </c>
+      <c r="D67" t="s">
+        <v>21</v>
+      </c>
+      <c r="E67" t="s">
+        <v>22</v>
+      </c>
+      <c r="F67" t="s">
+        <v>23</v>
+      </c>
+      <c r="G67" t="s">
+        <v>24</v>
+      </c>
+      <c r="H67" t="s">
+        <v>25</v>
+      </c>
+      <c r="I67" t="s">
+        <v>26</v>
+      </c>
+      <c r="J67" t="s">
+        <v>27</v>
+      </c>
+      <c r="K67" t="s">
+        <v>31</v>
+      </c>
+      <c r="L67" t="s">
+        <v>32</v>
+      </c>
+      <c r="M67" t="s">
+        <v>32</v>
+      </c>
+      <c r="N67" t="s">
+        <v>32</v>
+      </c>
+      <c r="O67" t="s">
+        <v>98</v>
+      </c>
+      <c r="P67" t="s">
+        <v>106</v>
+      </c>
+      <c r="T67" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="68" spans="1:20">
+      <c r="A68" s="1">
+        <v>66</v>
+      </c>
+      <c r="B68" t="s">
+        <v>19</v>
+      </c>
+      <c r="C68" t="s">
+        <v>20</v>
+      </c>
+      <c r="D68" t="s">
+        <v>21</v>
+      </c>
+      <c r="E68" t="s">
+        <v>22</v>
+      </c>
+      <c r="F68" t="s">
+        <v>23</v>
+      </c>
+      <c r="G68" t="s">
+        <v>24</v>
+      </c>
+      <c r="H68" t="s">
+        <v>25</v>
+      </c>
+      <c r="I68" t="s">
+        <v>26</v>
+      </c>
+      <c r="J68" t="s">
+        <v>27</v>
+      </c>
+      <c r="K68" t="s">
+        <v>31</v>
+      </c>
+      <c r="L68" t="s">
+        <v>32</v>
+      </c>
+      <c r="M68" t="s">
+        <v>32</v>
+      </c>
+      <c r="N68" t="s">
+        <v>32</v>
+      </c>
+      <c r="O68" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q68" t="s">
+        <v>113</v>
+      </c>
+      <c r="R68" t="s">
+        <v>119</v>
+      </c>
+      <c r="S68" t="s">
+        <v>132</v>
+      </c>
+      <c r="T68" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="69" spans="1:20">
+      <c r="A69" s="1">
+        <v>67</v>
+      </c>
+      <c r="B69" t="s">
+        <v>19</v>
+      </c>
+      <c r="C69" t="s">
+        <v>20</v>
+      </c>
+      <c r="D69" t="s">
+        <v>21</v>
+      </c>
+      <c r="E69" t="s">
+        <v>22</v>
+      </c>
+      <c r="F69" t="s">
+        <v>23</v>
+      </c>
+      <c r="G69" t="s">
+        <v>24</v>
+      </c>
+      <c r="H69" t="s">
+        <v>25</v>
+      </c>
+      <c r="I69" t="s">
+        <v>26</v>
+      </c>
+      <c r="J69" t="s">
+        <v>27</v>
+      </c>
+      <c r="K69" t="s">
+        <v>31</v>
+      </c>
+      <c r="L69" t="s">
+        <v>32</v>
+      </c>
+      <c r="M69" t="s">
+        <v>32</v>
+      </c>
+      <c r="N69" t="s">
+        <v>32</v>
+      </c>
+      <c r="O69" t="s">
+        <v>100</v>
+      </c>
+      <c r="Q69" t="s">
+        <v>112</v>
+      </c>
+      <c r="R69" t="s">
+        <v>119</v>
+      </c>
+      <c r="S69" t="s">
+        <v>129</v>
+      </c>
+      <c r="T69" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="70" spans="1:20">
+      <c r="A70" s="1">
+        <v>68</v>
+      </c>
+      <c r="B70" t="s">
+        <v>19</v>
+      </c>
+      <c r="C70" t="s">
+        <v>20</v>
+      </c>
+      <c r="D70" t="s">
+        <v>21</v>
+      </c>
+      <c r="E70" t="s">
+        <v>22</v>
+      </c>
+      <c r="F70" t="s">
+        <v>23</v>
+      </c>
+      <c r="G70" t="s">
+        <v>24</v>
+      </c>
+      <c r="H70" t="s">
+        <v>25</v>
+      </c>
+      <c r="I70" t="s">
+        <v>26</v>
+      </c>
+      <c r="J70" t="s">
+        <v>27</v>
+      </c>
+      <c r="K70" t="s">
+        <v>31</v>
+      </c>
+      <c r="L70" t="s">
+        <v>32</v>
+      </c>
+      <c r="M70" t="s">
+        <v>32</v>
+      </c>
+      <c r="N70" t="s">
+        <v>32</v>
+      </c>
+      <c r="O70" t="s">
+        <v>101</v>
+      </c>
+      <c r="T70" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="71" spans="1:20">
+      <c r="A71" s="1">
+        <v>69</v>
+      </c>
+      <c r="B71" t="s">
+        <v>19</v>
+      </c>
+      <c r="C71" t="s">
+        <v>20</v>
+      </c>
+      <c r="D71" t="s">
+        <v>21</v>
+      </c>
+      <c r="E71" t="s">
+        <v>22</v>
+      </c>
+      <c r="F71" t="s">
+        <v>23</v>
+      </c>
+      <c r="G71" t="s">
+        <v>24</v>
+      </c>
+      <c r="H71" t="s">
+        <v>25</v>
+      </c>
+      <c r="I71" t="s">
+        <v>26</v>
+      </c>
+      <c r="J71" t="s">
+        <v>27</v>
+      </c>
+      <c r="K71" t="s">
+        <v>31</v>
+      </c>
+      <c r="L71" t="s">
+        <v>32</v>
+      </c>
+      <c r="M71" t="s">
+        <v>32</v>
+      </c>
+      <c r="N71" t="s">
+        <v>32</v>
+      </c>
+      <c r="O71" t="s">
+        <v>102</v>
+      </c>
+      <c r="Q71" t="s">
+        <v>116</v>
+      </c>
+      <c r="R71" t="s">
+        <v>120</v>
+      </c>
+      <c r="S71" t="s">
+        <v>124</v>
+      </c>
+      <c r="T71" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="72" spans="1:20">
+      <c r="A72" s="1">
+        <v>70</v>
+      </c>
+      <c r="B72" t="s">
+        <v>19</v>
+      </c>
+      <c r="C72" t="s">
+        <v>20</v>
+      </c>
+      <c r="D72" t="s">
+        <v>21</v>
+      </c>
+      <c r="E72" t="s">
+        <v>22</v>
+      </c>
+      <c r="F72" t="s">
+        <v>23</v>
+      </c>
+      <c r="G72" t="s">
+        <v>24</v>
+      </c>
+      <c r="H72" t="s">
+        <v>25</v>
+      </c>
+      <c r="I72" t="s">
+        <v>26</v>
+      </c>
+      <c r="J72" t="s">
+        <v>27</v>
+      </c>
+      <c r="K72" t="s">
+        <v>31</v>
+      </c>
+      <c r="L72" t="s">
+        <v>32</v>
+      </c>
+      <c r="M72" t="s">
+        <v>32</v>
+      </c>
+      <c r="N72" t="s">
+        <v>32</v>
+      </c>
+      <c r="O72" t="s">
         <v>103</v>
       </c>
-      <c r="S61" t="s">
-        <v>105</v>
-      </c>
-      <c r="T61" t="s">
-        <v>172</v>
+      <c r="R72" t="s">
+        <v>120</v>
+      </c>
+      <c r="S72" t="s">
+        <v>131</v>
+      </c>
+      <c r="T72" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="73" spans="1:20">
+      <c r="A73" s="1">
+        <v>71</v>
+      </c>
+      <c r="B73" t="s">
+        <v>19</v>
+      </c>
+      <c r="C73" t="s">
+        <v>20</v>
+      </c>
+      <c r="D73" t="s">
+        <v>21</v>
+      </c>
+      <c r="E73" t="s">
+        <v>22</v>
+      </c>
+      <c r="F73" t="s">
+        <v>23</v>
+      </c>
+      <c r="G73" t="s">
+        <v>24</v>
+      </c>
+      <c r="H73" t="s">
+        <v>25</v>
+      </c>
+      <c r="I73" t="s">
+        <v>26</v>
+      </c>
+      <c r="J73" t="s">
+        <v>27</v>
+      </c>
+      <c r="K73" t="s">
+        <v>31</v>
+      </c>
+      <c r="L73" t="s">
+        <v>32</v>
+      </c>
+      <c r="M73" t="s">
+        <v>32</v>
+      </c>
+      <c r="N73" t="s">
+        <v>32</v>
+      </c>
+      <c r="O73" t="s">
+        <v>104</v>
+      </c>
+      <c r="T73" t="s">
+        <v>207</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D9BAEAB-D5D3-429C-BEF3-17AF3A9B0C83}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="AC26" sqref="AC26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Clean up moving the Items
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4937" uniqueCount="445">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4678" uniqueCount="448">
   <si>
     <t>individual</t>
   </si>
@@ -70,12 +70,12 @@
     <t>providedBy</t>
   </si>
   <si>
+    <t>items</t>
+  </si>
+  <si>
     <t>details</t>
   </si>
   <si>
-    <t>items</t>
-  </si>
-  <si>
     <t>GAN:MHB18-00032 / Alive / Male  / -</t>
   </si>
   <si>
@@ -524,6 +524,36 @@
   </si>
   <si>
     <t>Andrew Craton, Kim Boardman</t>
+  </si>
+  <si>
+    <t>bark chips, pinecones, field corn</t>
+  </si>
+  <si>
+    <t>sand, bark chips, mealworms, clementine wedges, chunks of pear</t>
+  </si>
+  <si>
+    <t>river rocks, water</t>
+  </si>
+  <si>
+    <t>river rocks, corn, water</t>
+  </si>
+  <si>
+    <t>sand, straw, gelatin cudes, mealworms, blueberries, peanuts</t>
+  </si>
+  <si>
+    <t>water, river rocks, cranberries, mealworms</t>
+  </si>
+  <si>
+    <t>sand, cranberries, mealworms, straw</t>
+  </si>
+  <si>
+    <t>bark chips, cranberries, mealworms</t>
+  </si>
+  <si>
+    <t>potato, shrimp, bark</t>
+  </si>
+  <si>
+    <t>top soil, field corn, apple, fir branches</t>
   </si>
   <si>
     <t>Items: bark chips, pinecones, field corn  
@@ -549,33 +579,37 @@
   </si>
   <si>
     <t>Items: sand, straw, gelatin cudes, mealworms, blueberries, peanuts
-Medium footbath with sand, straw, gelatin cubes with mealworms and blueberries and some peanuts.
+Description/ placement: Medium footbath with sand, straw, gelatin cubes with mealworms and blueberries and some peanuts.
 Removed:12/6 AV
 Eval: Straw strewn around, gelatin cubes gone, found peanut shells outside bowl, but peanuts eaten.</t>
   </si>
   <si>
     <t>Items: water, river rocks, cranberries, mealworms
-Medium sized footbath with water, river rocks, cranberries and mealworms.  Both over to enrichment right away and eating things.
+Description/ placement: Medium sized footbath with water, river rocks, cranberries and mealworms.  Both over to enrichment right away and eating things.
 Removed: 7 Jan 2020, MW
 Eval: Mealworms and cranberries were gone, rocks still in footbath with some frozen water.  Signs of frozen water splashed around ftbth.</t>
   </si>
   <si>
-    <t>large footbath with sand, some cranberries, mealworms and straw over top.
+    <t>Items: sand, cranberries, mealworms, straw
+Description/ placement: large footbath with sand, some cranberries, mealworms and straw over top.
 Removed:  15 Jan, KT
 Eval: Some straw pulled out of bowl and laying in snow.  Cranberries still present in bowl but no sign of mealworms.</t>
   </si>
   <si>
-    <t>Small treat bowl with bark chips, cranberries and mealworms placed in yard.
+    <t>Items:bark chips, cranberries, mealworms 
+Description/ placement: Small treat bowl with bark chips, cranberries and mealworms placed in yard.
 Removed:
 Eval:</t>
   </si>
   <si>
-    <t>Small treat bowl with potato and shrimp chunks under bark. (for Q Sarus two bowls). Placement: Niles-in house, Cj-Outside, Q Sarus- Inside.
+    <t>Items: potato, shrimp, bark
+Description/ placement: Small treat bowl with potato and shrimp chunks under bark. (for Q Sarus two bowls). Placement: Niles-in house, Cj-Outside, Q Sarus- Inside.
 Removed:
 Eval:</t>
   </si>
   <si>
-    <t>Medium sized footbath with top soil, field corn, some pieces of apple, covered with pieces of fir branches.
+    <t>Items: top soil, field corn, apple, fir branches
+Description/ placement: Medium sized footbath with top soil, field corn, some pieces of apple, covered with pieces of fir branches.
 Removed:
 Eval:</t>
   </si>
@@ -1834,37 +1868,6 @@
     <t>Description/ placement: treat bowl with lettuce, 1 tbsp  of sprouted seeds, and some mlws placed on E side of house
 Removed date/initials:
 Evaluation:</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> bark chips, pinecones, field corn  
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> sand, bark chips, mealworms, clementine wedges, chunks of pear
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> river rocks, water
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> river rocks, corn, water
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> sand, straw, gelatin cudes, mealworms, blueberries, peanuts
-Medium footbath with sand, straw, gelatin cubes with mealworms and blueberries and some peanuts.
-Removed:12/6 AV
-Eval: Straw strewn around, gelatin cubes gone, found peanut shells outside bowl, but peanuts eaten</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> water, river rocks, cranberries, mealworms
-Medium sized footbath with water, river rocks, cranberries and mealworms.  Both over to enrichment right away and eating things.
-Removed: 7 Jan 2020, MW
-Eval: Mealworms and cranberries were gone, rocks still in footbath with some frozen water.  Signs of frozen water splashed around ftbth</t>
-  </si>
-  <si>
-    <t>[]</t>
   </si>
 </sst>
 </file>
@@ -2346,7 +2349,7 @@
         <v>170</v>
       </c>
       <c r="U2" t="s">
-        <v>438</v>
+        <v>180</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -2411,7 +2414,7 @@
         <v>171</v>
       </c>
       <c r="U3" t="s">
-        <v>439</v>
+        <v>181</v>
       </c>
     </row>
     <row r="4" spans="1:21">
@@ -2464,7 +2467,7 @@
         <v>172</v>
       </c>
       <c r="U4" t="s">
-        <v>440</v>
+        <v>182</v>
       </c>
     </row>
     <row r="5" spans="1:21">
@@ -2529,7 +2532,7 @@
         <v>173</v>
       </c>
       <c r="U5" t="s">
-        <v>441</v>
+        <v>183</v>
       </c>
     </row>
     <row r="6" spans="1:21">
@@ -2594,7 +2597,7 @@
         <v>174</v>
       </c>
       <c r="U6" t="s">
-        <v>442</v>
+        <v>184</v>
       </c>
     </row>
     <row r="7" spans="1:21">
@@ -2659,7 +2662,7 @@
         <v>175</v>
       </c>
       <c r="U7" t="s">
-        <v>443</v>
+        <v>185</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -2724,7 +2727,7 @@
         <v>176</v>
       </c>
       <c r="U8" t="s">
-        <v>444</v>
+        <v>186</v>
       </c>
     </row>
     <row r="9" spans="1:21">
@@ -2777,7 +2780,7 @@
         <v>177</v>
       </c>
       <c r="U9" t="s">
-        <v>444</v>
+        <v>187</v>
       </c>
     </row>
     <row r="10" spans="1:21">
@@ -2833,7 +2836,7 @@
         <v>178</v>
       </c>
       <c r="U10" t="s">
-        <v>444</v>
+        <v>188</v>
       </c>
     </row>
     <row r="11" spans="1:21">
@@ -2889,7 +2892,7 @@
         <v>179</v>
       </c>
       <c r="U11" t="s">
-        <v>444</v>
+        <v>189</v>
       </c>
     </row>
     <row r="12" spans="1:21">
@@ -2947,11 +2950,8 @@
       <c r="S12" t="s">
         <v>157</v>
       </c>
-      <c r="T12" t="s">
-        <v>180</v>
-      </c>
       <c r="U12" t="s">
-        <v>444</v>
+        <v>190</v>
       </c>
     </row>
     <row r="13" spans="1:21">
@@ -3003,11 +3003,8 @@
       <c r="R13" t="s">
         <v>151</v>
       </c>
-      <c r="T13" t="s">
-        <v>181</v>
-      </c>
       <c r="U13" t="s">
-        <v>444</v>
+        <v>191</v>
       </c>
     </row>
     <row r="14" spans="1:21">
@@ -3062,11 +3059,8 @@
       <c r="S14" t="s">
         <v>155</v>
       </c>
-      <c r="T14" t="s">
-        <v>182</v>
-      </c>
       <c r="U14" t="s">
-        <v>444</v>
+        <v>192</v>
       </c>
     </row>
     <row r="15" spans="1:21">
@@ -3127,11 +3121,8 @@
       <c r="S15" t="s">
         <v>157</v>
       </c>
-      <c r="T15" t="s">
-        <v>183</v>
-      </c>
       <c r="U15" t="s">
-        <v>444</v>
+        <v>193</v>
       </c>
     </row>
     <row r="16" spans="1:21">
@@ -3186,11 +3177,8 @@
       <c r="S16" t="s">
         <v>158</v>
       </c>
-      <c r="T16" t="s">
-        <v>184</v>
-      </c>
       <c r="U16" t="s">
-        <v>444</v>
+        <v>194</v>
       </c>
     </row>
     <row r="17" spans="1:21">
@@ -3242,11 +3230,8 @@
       <c r="P17" t="s">
         <v>131</v>
       </c>
-      <c r="T17" t="s">
-        <v>185</v>
-      </c>
       <c r="U17" t="s">
-        <v>444</v>
+        <v>195</v>
       </c>
     </row>
     <row r="18" spans="1:21">
@@ -3295,11 +3280,8 @@
       <c r="O18" t="s">
         <v>71</v>
       </c>
-      <c r="T18" t="s">
-        <v>186</v>
-      </c>
       <c r="U18" t="s">
-        <v>444</v>
+        <v>196</v>
       </c>
     </row>
     <row r="19" spans="1:21">
@@ -3357,11 +3339,8 @@
       <c r="S19" t="s">
         <v>159</v>
       </c>
-      <c r="T19" t="s">
-        <v>187</v>
-      </c>
       <c r="U19" t="s">
-        <v>444</v>
+        <v>197</v>
       </c>
     </row>
     <row r="20" spans="1:21">
@@ -3422,11 +3401,8 @@
       <c r="S20" t="s">
         <v>158</v>
       </c>
-      <c r="T20" t="s">
-        <v>188</v>
-      </c>
       <c r="U20" t="s">
-        <v>444</v>
+        <v>198</v>
       </c>
     </row>
     <row r="21" spans="1:21">
@@ -3478,11 +3454,8 @@
       <c r="P21" t="s">
         <v>133</v>
       </c>
-      <c r="T21" t="s">
-        <v>189</v>
-      </c>
       <c r="U21" t="s">
-        <v>444</v>
+        <v>199</v>
       </c>
     </row>
     <row r="22" spans="1:21">
@@ -3534,11 +3507,8 @@
       <c r="P22" t="s">
         <v>132</v>
       </c>
-      <c r="T22" t="s">
-        <v>190</v>
-      </c>
       <c r="U22" t="s">
-        <v>444</v>
+        <v>200</v>
       </c>
     </row>
     <row r="23" spans="1:21">
@@ -3599,11 +3569,8 @@
       <c r="S23" t="s">
         <v>160</v>
       </c>
-      <c r="T23" t="s">
-        <v>191</v>
-      </c>
       <c r="U23" t="s">
-        <v>444</v>
+        <v>201</v>
       </c>
     </row>
     <row r="24" spans="1:21">
@@ -3664,11 +3631,8 @@
       <c r="S24" t="s">
         <v>156</v>
       </c>
-      <c r="T24" t="s">
-        <v>192</v>
-      </c>
       <c r="U24" t="s">
-        <v>444</v>
+        <v>202</v>
       </c>
     </row>
     <row r="25" spans="1:21">
@@ -3720,11 +3684,8 @@
       <c r="P25" t="s">
         <v>131</v>
       </c>
-      <c r="T25" t="s">
-        <v>193</v>
-      </c>
       <c r="U25" t="s">
-        <v>444</v>
+        <v>203</v>
       </c>
     </row>
     <row r="26" spans="1:21">
@@ -3773,11 +3734,8 @@
       <c r="O26" t="s">
         <v>79</v>
       </c>
-      <c r="T26" t="s">
-        <v>194</v>
-      </c>
       <c r="U26" t="s">
-        <v>444</v>
+        <v>204</v>
       </c>
     </row>
     <row r="27" spans="1:21">
@@ -3829,11 +3787,8 @@
       <c r="P27" t="s">
         <v>130</v>
       </c>
-      <c r="T27" t="s">
-        <v>195</v>
-      </c>
       <c r="U27" t="s">
-        <v>444</v>
+        <v>205</v>
       </c>
     </row>
     <row r="28" spans="1:21">
@@ -3885,11 +3840,8 @@
       <c r="P28" t="s">
         <v>131</v>
       </c>
-      <c r="T28" t="s">
-        <v>196</v>
-      </c>
       <c r="U28" t="s">
-        <v>444</v>
+        <v>206</v>
       </c>
     </row>
     <row r="29" spans="1:21">
@@ -3950,11 +3902,8 @@
       <c r="S29" t="s">
         <v>156</v>
       </c>
-      <c r="T29" t="s">
-        <v>197</v>
-      </c>
       <c r="U29" t="s">
-        <v>444</v>
+        <v>207</v>
       </c>
     </row>
     <row r="30" spans="1:21">
@@ -4009,11 +3958,8 @@
       <c r="S30" t="s">
         <v>155</v>
       </c>
-      <c r="T30" t="s">
-        <v>198</v>
-      </c>
       <c r="U30" t="s">
-        <v>444</v>
+        <v>208</v>
       </c>
     </row>
     <row r="31" spans="1:21">
@@ -4062,11 +4008,8 @@
       <c r="O31" t="s">
         <v>84</v>
       </c>
-      <c r="T31" t="s">
-        <v>199</v>
-      </c>
       <c r="U31" t="s">
-        <v>444</v>
+        <v>209</v>
       </c>
     </row>
     <row r="32" spans="1:21">
@@ -4115,11 +4058,8 @@
       <c r="O32" t="s">
         <v>85</v>
       </c>
-      <c r="T32" t="s">
-        <v>200</v>
-      </c>
       <c r="U32" t="s">
-        <v>444</v>
+        <v>210</v>
       </c>
     </row>
     <row r="33" spans="1:21">
@@ -4168,11 +4108,8 @@
       <c r="O33" t="s">
         <v>86</v>
       </c>
-      <c r="T33" t="s">
-        <v>201</v>
-      </c>
       <c r="U33" t="s">
-        <v>444</v>
+        <v>211</v>
       </c>
     </row>
     <row r="34" spans="1:21">
@@ -4230,11 +4167,8 @@
       <c r="S34" t="s">
         <v>161</v>
       </c>
-      <c r="T34" t="s">
-        <v>202</v>
-      </c>
       <c r="U34" t="s">
-        <v>444</v>
+        <v>212</v>
       </c>
     </row>
     <row r="35" spans="1:21">
@@ -4283,11 +4217,8 @@
       <c r="O35" t="s">
         <v>88</v>
       </c>
-      <c r="T35" t="s">
-        <v>203</v>
-      </c>
       <c r="U35" t="s">
-        <v>444</v>
+        <v>213</v>
       </c>
     </row>
     <row r="36" spans="1:21">
@@ -4339,11 +4270,8 @@
       <c r="Q36" t="s">
         <v>145</v>
       </c>
-      <c r="T36" t="s">
-        <v>204</v>
-      </c>
       <c r="U36" t="s">
-        <v>444</v>
+        <v>214</v>
       </c>
     </row>
     <row r="37" spans="1:21">
@@ -4404,11 +4332,8 @@
       <c r="S37" t="s">
         <v>155</v>
       </c>
-      <c r="T37" t="s">
-        <v>205</v>
-      </c>
       <c r="U37" t="s">
-        <v>444</v>
+        <v>215</v>
       </c>
     </row>
     <row r="38" spans="1:21">
@@ -4466,11 +4391,8 @@
       <c r="S38" t="s">
         <v>162</v>
       </c>
-      <c r="T38" t="s">
-        <v>206</v>
-      </c>
       <c r="U38" t="s">
-        <v>444</v>
+        <v>216</v>
       </c>
     </row>
     <row r="39" spans="1:21">
@@ -4519,11 +4441,8 @@
       <c r="O39" t="s">
         <v>92</v>
       </c>
-      <c r="T39" t="s">
-        <v>207</v>
-      </c>
       <c r="U39" t="s">
-        <v>444</v>
+        <v>217</v>
       </c>
     </row>
     <row r="40" spans="1:21">
@@ -4581,11 +4500,8 @@
       <c r="S40" t="s">
         <v>161</v>
       </c>
-      <c r="T40" t="s">
-        <v>208</v>
-      </c>
       <c r="U40" t="s">
-        <v>444</v>
+        <v>218</v>
       </c>
     </row>
     <row r="41" spans="1:21">
@@ -4634,11 +4550,8 @@
       <c r="O41" t="s">
         <v>94</v>
       </c>
-      <c r="T41" t="s">
-        <v>209</v>
-      </c>
       <c r="U41" t="s">
-        <v>444</v>
+        <v>219</v>
       </c>
     </row>
     <row r="42" spans="1:21">
@@ -4687,11 +4600,8 @@
       <c r="O42" t="s">
         <v>95</v>
       </c>
-      <c r="T42" t="s">
-        <v>210</v>
-      </c>
       <c r="U42" t="s">
-        <v>444</v>
+        <v>220</v>
       </c>
     </row>
     <row r="43" spans="1:21">
@@ -4749,11 +4659,8 @@
       <c r="S43" t="s">
         <v>163</v>
       </c>
-      <c r="T43" t="s">
-        <v>211</v>
-      </c>
       <c r="U43" t="s">
-        <v>444</v>
+        <v>221</v>
       </c>
     </row>
     <row r="44" spans="1:21">
@@ -4811,11 +4718,8 @@
       <c r="S44" t="s">
         <v>158</v>
       </c>
-      <c r="T44" t="s">
-        <v>212</v>
-      </c>
       <c r="U44" t="s">
-        <v>444</v>
+        <v>222</v>
       </c>
     </row>
     <row r="45" spans="1:21">
@@ -4867,11 +4771,8 @@
       <c r="Q45" t="s">
         <v>144</v>
       </c>
-      <c r="T45" t="s">
-        <v>213</v>
-      </c>
       <c r="U45" t="s">
-        <v>444</v>
+        <v>223</v>
       </c>
     </row>
     <row r="46" spans="1:21">
@@ -4920,11 +4821,8 @@
       <c r="O46" t="s">
         <v>99</v>
       </c>
-      <c r="T46" t="s">
-        <v>214</v>
-      </c>
       <c r="U46" t="s">
-        <v>444</v>
+        <v>224</v>
       </c>
     </row>
     <row r="47" spans="1:21">
@@ -4979,11 +4877,8 @@
       <c r="R47" t="s">
         <v>151</v>
       </c>
-      <c r="T47" t="s">
-        <v>215</v>
-      </c>
       <c r="U47" t="s">
-        <v>444</v>
+        <v>225</v>
       </c>
     </row>
     <row r="48" spans="1:21">
@@ -5044,11 +4939,8 @@
       <c r="S48" t="s">
         <v>157</v>
       </c>
-      <c r="T48" t="s">
-        <v>216</v>
-      </c>
       <c r="U48" t="s">
-        <v>444</v>
+        <v>226</v>
       </c>
     </row>
     <row r="49" spans="1:21">
@@ -5097,11 +4989,8 @@
       <c r="O49" t="s">
         <v>102</v>
       </c>
-      <c r="T49" t="s">
-        <v>217</v>
-      </c>
       <c r="U49" t="s">
-        <v>444</v>
+        <v>227</v>
       </c>
     </row>
     <row r="50" spans="1:21">
@@ -5150,11 +5039,8 @@
       <c r="O50" t="s">
         <v>103</v>
       </c>
-      <c r="T50" t="s">
-        <v>218</v>
-      </c>
       <c r="U50" t="s">
-        <v>444</v>
+        <v>228</v>
       </c>
     </row>
     <row r="51" spans="1:21">
@@ -5203,11 +5089,8 @@
       <c r="O51" t="s">
         <v>104</v>
       </c>
-      <c r="T51" t="s">
-        <v>219</v>
-      </c>
       <c r="U51" t="s">
-        <v>444</v>
+        <v>229</v>
       </c>
     </row>
     <row r="52" spans="1:21">
@@ -5256,11 +5139,8 @@
       <c r="O52" t="s">
         <v>105</v>
       </c>
-      <c r="T52" t="s">
-        <v>220</v>
-      </c>
       <c r="U52" t="s">
-        <v>444</v>
+        <v>230</v>
       </c>
     </row>
     <row r="53" spans="1:21">
@@ -5312,11 +5192,8 @@
       <c r="P53" t="s">
         <v>132</v>
       </c>
-      <c r="T53" t="s">
-        <v>221</v>
-      </c>
       <c r="U53" t="s">
-        <v>444</v>
+        <v>231</v>
       </c>
     </row>
     <row r="54" spans="1:21">
@@ -5368,11 +5245,8 @@
       <c r="P54" t="s">
         <v>131</v>
       </c>
-      <c r="T54" t="s">
-        <v>222</v>
-      </c>
       <c r="U54" t="s">
-        <v>444</v>
+        <v>232</v>
       </c>
     </row>
     <row r="55" spans="1:21">
@@ -5433,11 +5307,8 @@
       <c r="S55" t="s">
         <v>157</v>
       </c>
-      <c r="T55" t="s">
-        <v>223</v>
-      </c>
       <c r="U55" t="s">
-        <v>444</v>
+        <v>233</v>
       </c>
     </row>
     <row r="56" spans="1:21">
@@ -5486,11 +5357,8 @@
       <c r="O56" t="s">
         <v>109</v>
       </c>
-      <c r="T56" t="s">
-        <v>224</v>
-      </c>
       <c r="U56" t="s">
-        <v>444</v>
+        <v>234</v>
       </c>
     </row>
     <row r="57" spans="1:21">
@@ -5551,11 +5419,8 @@
       <c r="S57" t="s">
         <v>155</v>
       </c>
-      <c r="T57" t="s">
-        <v>225</v>
-      </c>
       <c r="U57" t="s">
-        <v>444</v>
+        <v>235</v>
       </c>
     </row>
     <row r="58" spans="1:21">
@@ -5616,11 +5481,8 @@
       <c r="S58" t="s">
         <v>164</v>
       </c>
-      <c r="T58" t="s">
-        <v>226</v>
-      </c>
       <c r="U58" t="s">
-        <v>444</v>
+        <v>236</v>
       </c>
     </row>
     <row r="59" spans="1:21">
@@ -5669,11 +5531,8 @@
       <c r="O59" t="s">
         <v>112</v>
       </c>
-      <c r="T59" t="s">
-        <v>227</v>
-      </c>
       <c r="U59" t="s">
-        <v>444</v>
+        <v>237</v>
       </c>
     </row>
     <row r="60" spans="1:21">
@@ -5722,11 +5581,8 @@
       <c r="O60" t="s">
         <v>113</v>
       </c>
-      <c r="T60" t="s">
-        <v>228</v>
-      </c>
       <c r="U60" t="s">
-        <v>444</v>
+        <v>238</v>
       </c>
     </row>
     <row r="61" spans="1:21">
@@ -5781,11 +5637,8 @@
       <c r="S61" t="s">
         <v>158</v>
       </c>
-      <c r="T61" t="s">
-        <v>229</v>
-      </c>
       <c r="U61" t="s">
-        <v>444</v>
+        <v>239</v>
       </c>
     </row>
     <row r="62" spans="1:21">
@@ -5834,11 +5687,8 @@
       <c r="O62" t="s">
         <v>115</v>
       </c>
-      <c r="T62" t="s">
-        <v>230</v>
-      </c>
       <c r="U62" t="s">
-        <v>444</v>
+        <v>240</v>
       </c>
     </row>
     <row r="63" spans="1:21">
@@ -5887,11 +5737,8 @@
       <c r="O63" t="s">
         <v>116</v>
       </c>
-      <c r="T63" t="s">
-        <v>231</v>
-      </c>
       <c r="U63" t="s">
-        <v>444</v>
+        <v>241</v>
       </c>
     </row>
     <row r="64" spans="1:21">
@@ -5946,11 +5793,8 @@
       <c r="S64" t="s">
         <v>158</v>
       </c>
-      <c r="T64" t="s">
-        <v>232</v>
-      </c>
       <c r="U64" t="s">
-        <v>444</v>
+        <v>242</v>
       </c>
     </row>
     <row r="65" spans="1:21">
@@ -6005,11 +5849,8 @@
       <c r="S65" t="s">
         <v>163</v>
       </c>
-      <c r="T65" t="s">
-        <v>233</v>
-      </c>
       <c r="U65" t="s">
-        <v>444</v>
+        <v>243</v>
       </c>
     </row>
     <row r="66" spans="1:21">
@@ -6058,11 +5899,8 @@
       <c r="O66" t="s">
         <v>119</v>
       </c>
-      <c r="T66" t="s">
-        <v>234</v>
-      </c>
       <c r="U66" t="s">
-        <v>444</v>
+        <v>244</v>
       </c>
     </row>
     <row r="67" spans="1:21">
@@ -6117,11 +5955,8 @@
       <c r="S67" t="s">
         <v>157</v>
       </c>
-      <c r="T67" t="s">
-        <v>235</v>
-      </c>
       <c r="U67" t="s">
-        <v>444</v>
+        <v>245</v>
       </c>
     </row>
     <row r="68" spans="1:21">
@@ -6176,11 +6011,8 @@
       <c r="S68" t="s">
         <v>161</v>
       </c>
-      <c r="T68" t="s">
-        <v>236</v>
-      </c>
       <c r="U68" t="s">
-        <v>444</v>
+        <v>246</v>
       </c>
     </row>
     <row r="69" spans="1:21">
@@ -6229,11 +6061,8 @@
       <c r="O69" t="s">
         <v>122</v>
       </c>
-      <c r="T69" t="s">
-        <v>237</v>
-      </c>
       <c r="U69" t="s">
-        <v>444</v>
+        <v>247</v>
       </c>
     </row>
     <row r="70" spans="1:21">
@@ -6282,11 +6111,8 @@
       <c r="O70" t="s">
         <v>123</v>
       </c>
-      <c r="T70" t="s">
-        <v>238</v>
-      </c>
       <c r="U70" t="s">
-        <v>444</v>
+        <v>248</v>
       </c>
     </row>
     <row r="71" spans="1:21">
@@ -6335,11 +6161,8 @@
       <c r="O71" t="s">
         <v>124</v>
       </c>
-      <c r="T71" t="s">
-        <v>239</v>
-      </c>
       <c r="U71" t="s">
-        <v>444</v>
+        <v>249</v>
       </c>
     </row>
     <row r="72" spans="1:21">
@@ -6394,11 +6217,8 @@
       <c r="S72" t="s">
         <v>160</v>
       </c>
-      <c r="T72" t="s">
-        <v>240</v>
-      </c>
       <c r="U72" t="s">
-        <v>444</v>
+        <v>250</v>
       </c>
     </row>
     <row r="73" spans="1:21">
@@ -6459,11 +6279,8 @@
       <c r="S73" t="s">
         <v>155</v>
       </c>
-      <c r="T73" t="s">
-        <v>241</v>
-      </c>
       <c r="U73" t="s">
-        <v>444</v>
+        <v>251</v>
       </c>
     </row>
     <row r="74" spans="1:21">
@@ -6524,11 +6341,8 @@
       <c r="S74" t="s">
         <v>155</v>
       </c>
-      <c r="T74" t="s">
-        <v>242</v>
-      </c>
       <c r="U74" t="s">
-        <v>444</v>
+        <v>252</v>
       </c>
     </row>
     <row r="75" spans="1:21">
@@ -6589,11 +6403,8 @@
       <c r="S75" t="s">
         <v>160</v>
       </c>
-      <c r="T75" t="s">
-        <v>243</v>
-      </c>
       <c r="U75" t="s">
-        <v>444</v>
+        <v>253</v>
       </c>
     </row>
     <row r="76" spans="1:21">
@@ -6654,11 +6465,8 @@
       <c r="S76" t="s">
         <v>160</v>
       </c>
-      <c r="T76" t="s">
-        <v>244</v>
-      </c>
       <c r="U76" t="s">
-        <v>444</v>
+        <v>254</v>
       </c>
     </row>
     <row r="77" spans="1:21">
@@ -6719,11 +6527,8 @@
       <c r="S77" t="s">
         <v>155</v>
       </c>
-      <c r="T77" t="s">
-        <v>245</v>
-      </c>
       <c r="U77" t="s">
-        <v>444</v>
+        <v>255</v>
       </c>
     </row>
     <row r="78" spans="1:21">
@@ -6784,11 +6589,8 @@
       <c r="S78" t="s">
         <v>160</v>
       </c>
-      <c r="T78" t="s">
-        <v>246</v>
-      </c>
       <c r="U78" t="s">
-        <v>444</v>
+        <v>256</v>
       </c>
     </row>
     <row r="79" spans="1:21">
@@ -6849,11 +6651,8 @@
       <c r="S79" t="s">
         <v>160</v>
       </c>
-      <c r="T79" t="s">
-        <v>247</v>
-      </c>
       <c r="U79" t="s">
-        <v>444</v>
+        <v>257</v>
       </c>
     </row>
     <row r="80" spans="1:21">
@@ -6911,11 +6710,8 @@
       <c r="S80" t="s">
         <v>158</v>
       </c>
-      <c r="T80" t="s">
-        <v>248</v>
-      </c>
       <c r="U80" t="s">
-        <v>444</v>
+        <v>258</v>
       </c>
     </row>
     <row r="81" spans="1:21">
@@ -6976,11 +6772,8 @@
       <c r="S81" t="s">
         <v>155</v>
       </c>
-      <c r="T81" t="s">
-        <v>249</v>
-      </c>
       <c r="U81" t="s">
-        <v>444</v>
+        <v>259</v>
       </c>
     </row>
     <row r="82" spans="1:21">
@@ -7041,11 +6834,8 @@
       <c r="S82" t="s">
         <v>155</v>
       </c>
-      <c r="T82" t="s">
-        <v>250</v>
-      </c>
       <c r="U82" t="s">
-        <v>444</v>
+        <v>260</v>
       </c>
     </row>
     <row r="83" spans="1:21">
@@ -7106,11 +6896,8 @@
       <c r="S83" t="s">
         <v>165</v>
       </c>
-      <c r="T83" t="s">
-        <v>251</v>
-      </c>
       <c r="U83" t="s">
-        <v>444</v>
+        <v>261</v>
       </c>
     </row>
     <row r="84" spans="1:21">
@@ -7159,11 +6946,8 @@
       <c r="O84" t="s">
         <v>101</v>
       </c>
-      <c r="T84" t="s">
-        <v>252</v>
-      </c>
       <c r="U84" t="s">
-        <v>444</v>
+        <v>262</v>
       </c>
     </row>
     <row r="85" spans="1:21">
@@ -7224,11 +7008,8 @@
       <c r="S85" t="s">
         <v>155</v>
       </c>
-      <c r="T85" t="s">
-        <v>253</v>
-      </c>
       <c r="U85" t="s">
-        <v>444</v>
+        <v>263</v>
       </c>
     </row>
     <row r="86" spans="1:21">
@@ -7286,11 +7067,8 @@
       <c r="S86" t="s">
         <v>159</v>
       </c>
-      <c r="T86" t="s">
-        <v>254</v>
-      </c>
       <c r="U86" t="s">
-        <v>444</v>
+        <v>264</v>
       </c>
     </row>
     <row r="87" spans="1:21">
@@ -7339,11 +7117,8 @@
       <c r="O87" t="s">
         <v>107</v>
       </c>
-      <c r="T87" t="s">
-        <v>255</v>
-      </c>
       <c r="U87" t="s">
-        <v>444</v>
+        <v>265</v>
       </c>
     </row>
     <row r="88" spans="1:21">
@@ -7398,11 +7173,8 @@
       <c r="R88" t="s">
         <v>150</v>
       </c>
-      <c r="T88" t="s">
-        <v>256</v>
-      </c>
       <c r="U88" t="s">
-        <v>444</v>
+        <v>266</v>
       </c>
     </row>
     <row r="89" spans="1:21">
@@ -7451,11 +7223,8 @@
       <c r="O89" t="s">
         <v>111</v>
       </c>
-      <c r="T89" t="s">
-        <v>257</v>
-      </c>
       <c r="U89" t="s">
-        <v>444</v>
+        <v>267</v>
       </c>
     </row>
     <row r="90" spans="1:21">
@@ -7504,11 +7273,8 @@
       <c r="O90" t="s">
         <v>111</v>
       </c>
-      <c r="T90" t="s">
-        <v>258</v>
-      </c>
       <c r="U90" t="s">
-        <v>444</v>
+        <v>268</v>
       </c>
     </row>
     <row r="91" spans="1:21">
@@ -7569,11 +7335,8 @@
       <c r="S91" t="s">
         <v>155</v>
       </c>
-      <c r="T91" t="s">
-        <v>259</v>
-      </c>
       <c r="U91" t="s">
-        <v>444</v>
+        <v>269</v>
       </c>
     </row>
     <row r="92" spans="1:21">
@@ -7625,11 +7388,8 @@
       <c r="P92" t="s">
         <v>131</v>
       </c>
-      <c r="T92" t="s">
-        <v>260</v>
-      </c>
       <c r="U92" t="s">
-        <v>444</v>
+        <v>270</v>
       </c>
     </row>
     <row r="93" spans="1:21">
@@ -7690,11 +7450,8 @@
       <c r="S93" t="s">
         <v>160</v>
       </c>
-      <c r="T93" t="s">
-        <v>261</v>
-      </c>
       <c r="U93" t="s">
-        <v>444</v>
+        <v>271</v>
       </c>
     </row>
     <row r="94" spans="1:21">
@@ -7755,11 +7512,8 @@
       <c r="S94" t="s">
         <v>160</v>
       </c>
-      <c r="T94" t="s">
-        <v>262</v>
-      </c>
       <c r="U94" t="s">
-        <v>444</v>
+        <v>272</v>
       </c>
     </row>
     <row r="95" spans="1:21">
@@ -7811,11 +7565,8 @@
       <c r="P95" t="s">
         <v>132</v>
       </c>
-      <c r="T95" t="s">
-        <v>263</v>
-      </c>
       <c r="U95" t="s">
-        <v>444</v>
+        <v>273</v>
       </c>
     </row>
     <row r="96" spans="1:21">
@@ -7873,11 +7624,8 @@
       <c r="S96" t="s">
         <v>160</v>
       </c>
-      <c r="T96" t="s">
-        <v>264</v>
-      </c>
       <c r="U96" t="s">
-        <v>444</v>
+        <v>274</v>
       </c>
     </row>
     <row r="97" spans="1:21">
@@ -7935,11 +7683,8 @@
       <c r="S97" t="s">
         <v>160</v>
       </c>
-      <c r="T97" t="s">
-        <v>265</v>
-      </c>
       <c r="U97" t="s">
-        <v>444</v>
+        <v>275</v>
       </c>
     </row>
     <row r="98" spans="1:21">
@@ -7997,11 +7742,8 @@
       <c r="S98" t="s">
         <v>160</v>
       </c>
-      <c r="T98" t="s">
-        <v>266</v>
-      </c>
       <c r="U98" t="s">
-        <v>444</v>
+        <v>276</v>
       </c>
     </row>
     <row r="99" spans="1:21">
@@ -8059,11 +7801,8 @@
       <c r="S99" t="s">
         <v>160</v>
       </c>
-      <c r="T99" t="s">
-        <v>267</v>
-      </c>
       <c r="U99" t="s">
-        <v>444</v>
+        <v>277</v>
       </c>
     </row>
     <row r="100" spans="1:21">
@@ -8112,11 +7851,8 @@
       <c r="O100" t="s">
         <v>72</v>
       </c>
-      <c r="T100" t="s">
-        <v>268</v>
-      </c>
       <c r="U100" t="s">
-        <v>444</v>
+        <v>278</v>
       </c>
     </row>
     <row r="101" spans="1:21">
@@ -8168,11 +7904,8 @@
       <c r="P101" t="s">
         <v>130</v>
       </c>
-      <c r="T101" t="s">
-        <v>269</v>
-      </c>
       <c r="U101" t="s">
-        <v>444</v>
+        <v>279</v>
       </c>
     </row>
     <row r="102" spans="1:21">
@@ -8230,11 +7963,8 @@
       <c r="R102" t="s">
         <v>150</v>
       </c>
-      <c r="T102" t="s">
-        <v>270</v>
-      </c>
       <c r="U102" t="s">
-        <v>444</v>
+        <v>280</v>
       </c>
     </row>
     <row r="103" spans="1:21">
@@ -8295,11 +8025,8 @@
       <c r="S103" t="s">
         <v>160</v>
       </c>
-      <c r="T103" t="s">
-        <v>271</v>
-      </c>
       <c r="U103" t="s">
-        <v>444</v>
+        <v>281</v>
       </c>
     </row>
     <row r="104" spans="1:21">
@@ -8354,11 +8081,8 @@
       <c r="Q104" t="s">
         <v>144</v>
       </c>
-      <c r="T104" t="s">
-        <v>272</v>
-      </c>
       <c r="U104" t="s">
-        <v>444</v>
+        <v>282</v>
       </c>
     </row>
     <row r="105" spans="1:21">
@@ -8419,11 +8143,8 @@
       <c r="S105" t="s">
         <v>160</v>
       </c>
-      <c r="T105" t="s">
-        <v>273</v>
-      </c>
       <c r="U105" t="s">
-        <v>444</v>
+        <v>283</v>
       </c>
     </row>
     <row r="106" spans="1:21">
@@ -8475,11 +8196,8 @@
       <c r="P106" t="s">
         <v>132</v>
       </c>
-      <c r="T106" t="s">
-        <v>274</v>
-      </c>
       <c r="U106" t="s">
-        <v>444</v>
+        <v>284</v>
       </c>
     </row>
     <row r="107" spans="1:21">
@@ -8528,11 +8246,8 @@
       <c r="O107" t="s">
         <v>99</v>
       </c>
-      <c r="T107" t="s">
-        <v>275</v>
-      </c>
       <c r="U107" t="s">
-        <v>444</v>
+        <v>285</v>
       </c>
     </row>
     <row r="108" spans="1:21">
@@ -8593,11 +8308,8 @@
       <c r="S108" t="s">
         <v>155</v>
       </c>
-      <c r="T108" t="s">
-        <v>276</v>
-      </c>
       <c r="U108" t="s">
-        <v>444</v>
+        <v>286</v>
       </c>
     </row>
     <row r="109" spans="1:21">
@@ -8655,11 +8367,8 @@
       <c r="S109" t="s">
         <v>165</v>
       </c>
-      <c r="T109" t="s">
-        <v>277</v>
-      </c>
       <c r="U109" t="s">
-        <v>444</v>
+        <v>287</v>
       </c>
     </row>
     <row r="110" spans="1:21">
@@ -8708,11 +8417,8 @@
       <c r="O110" t="s">
         <v>108</v>
       </c>
-      <c r="T110" t="s">
-        <v>278</v>
-      </c>
       <c r="U110" t="s">
-        <v>444</v>
+        <v>288</v>
       </c>
     </row>
     <row r="111" spans="1:21">
@@ -8773,11 +8479,8 @@
       <c r="S111" t="s">
         <v>155</v>
       </c>
-      <c r="T111" t="s">
-        <v>279</v>
-      </c>
       <c r="U111" t="s">
-        <v>444</v>
+        <v>289</v>
       </c>
     </row>
     <row r="112" spans="1:21">
@@ -8826,11 +8529,8 @@
       <c r="O112" t="s">
         <v>112</v>
       </c>
-      <c r="T112" t="s">
-        <v>280</v>
-      </c>
       <c r="U112" t="s">
-        <v>444</v>
+        <v>290</v>
       </c>
     </row>
     <row r="113" spans="1:21">
@@ -8891,11 +8591,8 @@
       <c r="S113" t="s">
         <v>155</v>
       </c>
-      <c r="T113" t="s">
-        <v>281</v>
-      </c>
       <c r="U113" t="s">
-        <v>444</v>
+        <v>291</v>
       </c>
     </row>
     <row r="114" spans="1:21">
@@ -8956,11 +8653,8 @@
       <c r="S114" t="s">
         <v>166</v>
       </c>
-      <c r="T114" t="s">
-        <v>282</v>
-      </c>
       <c r="U114" t="s">
-        <v>444</v>
+        <v>292</v>
       </c>
     </row>
     <row r="115" spans="1:21">
@@ -9021,11 +8715,8 @@
       <c r="S115" t="s">
         <v>155</v>
       </c>
-      <c r="T115" t="s">
-        <v>283</v>
-      </c>
       <c r="U115" t="s">
-        <v>444</v>
+        <v>293</v>
       </c>
     </row>
     <row r="116" spans="1:21">
@@ -9086,11 +8777,8 @@
       <c r="S116" t="s">
         <v>155</v>
       </c>
-      <c r="T116" t="s">
-        <v>284</v>
-      </c>
       <c r="U116" t="s">
-        <v>444</v>
+        <v>294</v>
       </c>
     </row>
     <row r="117" spans="1:21">
@@ -9151,11 +8839,8 @@
       <c r="S117" t="s">
         <v>162</v>
       </c>
-      <c r="T117" t="s">
-        <v>285</v>
-      </c>
       <c r="U117" t="s">
-        <v>444</v>
+        <v>295</v>
       </c>
     </row>
     <row r="118" spans="1:21">
@@ -9216,11 +8901,8 @@
       <c r="S118" t="s">
         <v>155</v>
       </c>
-      <c r="T118" t="s">
-        <v>286</v>
-      </c>
       <c r="U118" t="s">
-        <v>444</v>
+        <v>296</v>
       </c>
     </row>
     <row r="119" spans="1:21">
@@ -9281,11 +8963,8 @@
       <c r="S119" t="s">
         <v>159</v>
       </c>
-      <c r="T119" t="s">
-        <v>287</v>
-      </c>
       <c r="U119" t="s">
-        <v>444</v>
+        <v>297</v>
       </c>
     </row>
     <row r="120" spans="1:21">
@@ -9346,11 +9025,8 @@
       <c r="S120" t="s">
         <v>155</v>
       </c>
-      <c r="T120" t="s">
-        <v>288</v>
-      </c>
       <c r="U120" t="s">
-        <v>444</v>
+        <v>298</v>
       </c>
     </row>
     <row r="121" spans="1:21">
@@ -9408,11 +9084,8 @@
       <c r="S121" t="s">
         <v>162</v>
       </c>
-      <c r="T121" t="s">
-        <v>289</v>
-      </c>
       <c r="U121" t="s">
-        <v>444</v>
+        <v>299</v>
       </c>
     </row>
     <row r="122" spans="1:21">
@@ -9473,11 +9146,8 @@
       <c r="S122" t="s">
         <v>157</v>
       </c>
-      <c r="T122" t="s">
-        <v>290</v>
-      </c>
       <c r="U122" t="s">
-        <v>444</v>
+        <v>300</v>
       </c>
     </row>
     <row r="123" spans="1:21">
@@ -9535,11 +9205,8 @@
       <c r="S123" t="s">
         <v>163</v>
       </c>
-      <c r="T123" t="s">
-        <v>291</v>
-      </c>
       <c r="U123" t="s">
-        <v>444</v>
+        <v>301</v>
       </c>
     </row>
     <row r="124" spans="1:21">
@@ -9588,11 +9255,8 @@
       <c r="O124" t="s">
         <v>96</v>
       </c>
-      <c r="T124" t="s">
-        <v>292</v>
-      </c>
       <c r="U124" t="s">
-        <v>444</v>
+        <v>302</v>
       </c>
     </row>
     <row r="125" spans="1:21">
@@ -9641,11 +9305,8 @@
       <c r="O125" t="s">
         <v>128</v>
       </c>
-      <c r="T125" t="s">
-        <v>293</v>
-      </c>
       <c r="U125" t="s">
-        <v>444</v>
+        <v>303</v>
       </c>
     </row>
     <row r="126" spans="1:21">
@@ -9703,11 +9364,8 @@
       <c r="S126" t="s">
         <v>158</v>
       </c>
-      <c r="T126" t="s">
-        <v>294</v>
-      </c>
       <c r="U126" t="s">
-        <v>444</v>
+        <v>304</v>
       </c>
     </row>
     <row r="127" spans="1:21">
@@ -9765,11 +9423,8 @@
       <c r="S127" t="s">
         <v>159</v>
       </c>
-      <c r="T127" t="s">
-        <v>295</v>
-      </c>
       <c r="U127" t="s">
-        <v>444</v>
+        <v>305</v>
       </c>
     </row>
     <row r="128" spans="1:21">
@@ -9830,11 +9485,8 @@
       <c r="S128" t="s">
         <v>160</v>
       </c>
-      <c r="T128" t="s">
-        <v>296</v>
-      </c>
       <c r="U128" t="s">
-        <v>444</v>
+        <v>306</v>
       </c>
     </row>
     <row r="129" spans="1:21">
@@ -9892,11 +9544,8 @@
       <c r="S129" t="s">
         <v>158</v>
       </c>
-      <c r="T129" t="s">
-        <v>297</v>
-      </c>
       <c r="U129" t="s">
-        <v>444</v>
+        <v>307</v>
       </c>
     </row>
     <row r="130" spans="1:21">
@@ -9945,11 +9594,8 @@
       <c r="O130" t="s">
         <v>62</v>
       </c>
-      <c r="T130" t="s">
-        <v>298</v>
-      </c>
       <c r="U130" t="s">
-        <v>444</v>
+        <v>308</v>
       </c>
     </row>
     <row r="131" spans="1:21">
@@ -10007,11 +9653,8 @@
       <c r="S131" t="s">
         <v>155</v>
       </c>
-      <c r="T131" t="s">
-        <v>299</v>
-      </c>
       <c r="U131" t="s">
-        <v>444</v>
+        <v>309</v>
       </c>
     </row>
     <row r="132" spans="1:21">
@@ -10063,11 +9706,8 @@
       <c r="P132" t="s">
         <v>135</v>
       </c>
-      <c r="T132" t="s">
-        <v>300</v>
-      </c>
       <c r="U132" t="s">
-        <v>444</v>
+        <v>310</v>
       </c>
     </row>
     <row r="133" spans="1:21">
@@ -10128,11 +9768,8 @@
       <c r="S133" t="s">
         <v>157</v>
       </c>
-      <c r="T133" t="s">
-        <v>301</v>
-      </c>
       <c r="U133" t="s">
-        <v>444</v>
+        <v>311</v>
       </c>
     </row>
     <row r="134" spans="1:21">
@@ -10193,11 +9830,8 @@
       <c r="S134" t="s">
         <v>155</v>
       </c>
-      <c r="T134" t="s">
-        <v>302</v>
-      </c>
       <c r="U134" t="s">
-        <v>444</v>
+        <v>312</v>
       </c>
     </row>
     <row r="135" spans="1:21">
@@ -10255,11 +9889,8 @@
       <c r="S135" t="s">
         <v>158</v>
       </c>
-      <c r="T135" t="s">
-        <v>303</v>
-      </c>
       <c r="U135" t="s">
-        <v>444</v>
+        <v>313</v>
       </c>
     </row>
     <row r="136" spans="1:21">
@@ -10320,11 +9951,8 @@
       <c r="S136" t="s">
         <v>157</v>
       </c>
-      <c r="T136" t="s">
-        <v>304</v>
-      </c>
       <c r="U136" t="s">
-        <v>444</v>
+        <v>314</v>
       </c>
     </row>
     <row r="137" spans="1:21">
@@ -10373,11 +10001,8 @@
       <c r="O137" t="s">
         <v>65</v>
       </c>
-      <c r="T137" t="s">
-        <v>305</v>
-      </c>
       <c r="U137" t="s">
-        <v>444</v>
+        <v>315</v>
       </c>
     </row>
     <row r="138" spans="1:21">
@@ -10426,11 +10051,8 @@
       <c r="O138" t="s">
         <v>66</v>
       </c>
-      <c r="T138" t="s">
-        <v>306</v>
-      </c>
       <c r="U138" t="s">
-        <v>444</v>
+        <v>316</v>
       </c>
     </row>
     <row r="139" spans="1:21">
@@ -10482,11 +10104,8 @@
       <c r="P139" t="s">
         <v>136</v>
       </c>
-      <c r="T139" t="s">
-        <v>307</v>
-      </c>
       <c r="U139" t="s">
-        <v>444</v>
+        <v>317</v>
       </c>
     </row>
     <row r="140" spans="1:21">
@@ -10547,11 +10166,8 @@
       <c r="S140" t="s">
         <v>155</v>
       </c>
-      <c r="T140" t="s">
-        <v>308</v>
-      </c>
       <c r="U140" t="s">
-        <v>444</v>
+        <v>318</v>
       </c>
     </row>
     <row r="141" spans="1:21">
@@ -10603,11 +10219,8 @@
       <c r="P141" t="s">
         <v>134</v>
       </c>
-      <c r="T141" t="s">
-        <v>309</v>
-      </c>
       <c r="U141" t="s">
-        <v>444</v>
+        <v>319</v>
       </c>
     </row>
     <row r="142" spans="1:21">
@@ -10662,11 +10275,8 @@
       <c r="S142" t="s">
         <v>165</v>
       </c>
-      <c r="T142" t="s">
-        <v>310</v>
-      </c>
       <c r="U142" t="s">
-        <v>444</v>
+        <v>320</v>
       </c>
     </row>
     <row r="143" spans="1:21">
@@ -10727,11 +10337,8 @@
       <c r="S143" t="s">
         <v>162</v>
       </c>
-      <c r="T143" t="s">
-        <v>311</v>
-      </c>
       <c r="U143" t="s">
-        <v>444</v>
+        <v>321</v>
       </c>
     </row>
     <row r="144" spans="1:21">
@@ -10792,11 +10399,8 @@
       <c r="S144" t="s">
         <v>157</v>
       </c>
-      <c r="T144" t="s">
-        <v>312</v>
-      </c>
       <c r="U144" t="s">
-        <v>444</v>
+        <v>322</v>
       </c>
     </row>
     <row r="145" spans="1:21">
@@ -10857,11 +10461,8 @@
       <c r="S145" t="s">
         <v>167</v>
       </c>
-      <c r="T145" t="s">
-        <v>313</v>
-      </c>
       <c r="U145" t="s">
-        <v>444</v>
+        <v>323</v>
       </c>
     </row>
     <row r="146" spans="1:21">
@@ -10922,11 +10523,8 @@
       <c r="S146" t="s">
         <v>168</v>
       </c>
-      <c r="T146" t="s">
-        <v>314</v>
-      </c>
       <c r="U146" t="s">
-        <v>444</v>
+        <v>324</v>
       </c>
     </row>
     <row r="147" spans="1:21">
@@ -10987,11 +10585,8 @@
       <c r="S147" t="s">
         <v>169</v>
       </c>
-      <c r="T147" t="s">
-        <v>315</v>
-      </c>
       <c r="U147" t="s">
-        <v>444</v>
+        <v>325</v>
       </c>
     </row>
     <row r="148" spans="1:21">
@@ -11052,11 +10647,8 @@
       <c r="S148" t="s">
         <v>163</v>
       </c>
-      <c r="T148" t="s">
-        <v>316</v>
-      </c>
       <c r="U148" t="s">
-        <v>444</v>
+        <v>326</v>
       </c>
     </row>
     <row r="149" spans="1:21">
@@ -11117,11 +10709,8 @@
       <c r="S149" t="s">
         <v>158</v>
       </c>
-      <c r="T149" t="s">
-        <v>317</v>
-      </c>
       <c r="U149" t="s">
-        <v>444</v>
+        <v>327</v>
       </c>
     </row>
     <row r="150" spans="1:21">
@@ -11173,11 +10762,8 @@
       <c r="P150" t="s">
         <v>136</v>
       </c>
-      <c r="T150" t="s">
-        <v>318</v>
-      </c>
       <c r="U150" t="s">
-        <v>444</v>
+        <v>328</v>
       </c>
     </row>
     <row r="151" spans="1:21">
@@ -11238,11 +10824,8 @@
       <c r="S151" t="s">
         <v>160</v>
       </c>
-      <c r="T151" t="s">
-        <v>319</v>
-      </c>
       <c r="U151" t="s">
-        <v>444</v>
+        <v>329</v>
       </c>
     </row>
     <row r="152" spans="1:21">
@@ -11303,11 +10886,8 @@
       <c r="S152" t="s">
         <v>167</v>
       </c>
-      <c r="T152" t="s">
-        <v>320</v>
-      </c>
       <c r="U152" t="s">
-        <v>444</v>
+        <v>330</v>
       </c>
     </row>
     <row r="153" spans="1:21">
@@ -11359,11 +10939,8 @@
       <c r="P153" t="s">
         <v>131</v>
       </c>
-      <c r="T153" t="s">
-        <v>321</v>
-      </c>
       <c r="U153" t="s">
-        <v>444</v>
+        <v>331</v>
       </c>
     </row>
     <row r="154" spans="1:21">
@@ -11424,11 +11001,8 @@
       <c r="S154" t="s">
         <v>160</v>
       </c>
-      <c r="T154" t="s">
-        <v>322</v>
-      </c>
       <c r="U154" t="s">
-        <v>444</v>
+        <v>332</v>
       </c>
     </row>
     <row r="155" spans="1:21">
@@ -11489,11 +11063,8 @@
       <c r="S155" t="s">
         <v>157</v>
       </c>
-      <c r="T155" t="s">
-        <v>323</v>
-      </c>
       <c r="U155" t="s">
-        <v>444</v>
+        <v>333</v>
       </c>
     </row>
     <row r="156" spans="1:21">
@@ -11551,11 +11122,8 @@
       <c r="S156" t="s">
         <v>155</v>
       </c>
-      <c r="T156" t="s">
-        <v>324</v>
-      </c>
       <c r="U156" t="s">
-        <v>444</v>
+        <v>334</v>
       </c>
     </row>
     <row r="157" spans="1:21">
@@ -11613,11 +11181,8 @@
       <c r="S157" t="s">
         <v>165</v>
       </c>
-      <c r="T157" t="s">
-        <v>325</v>
-      </c>
       <c r="U157" t="s">
-        <v>444</v>
+        <v>335</v>
       </c>
     </row>
     <row r="158" spans="1:21">
@@ -11669,11 +11234,8 @@
       <c r="P158" t="s">
         <v>137</v>
       </c>
-      <c r="T158" t="s">
-        <v>326</v>
-      </c>
       <c r="U158" t="s">
-        <v>444</v>
+        <v>336</v>
       </c>
     </row>
     <row r="159" spans="1:21">
@@ -11725,11 +11287,8 @@
       <c r="P159" t="s">
         <v>133</v>
       </c>
-      <c r="T159" t="s">
-        <v>327</v>
-      </c>
       <c r="U159" t="s">
-        <v>444</v>
+        <v>337</v>
       </c>
     </row>
     <row r="160" spans="1:21">
@@ -11787,11 +11346,8 @@
       <c r="S160" t="s">
         <v>165</v>
       </c>
-      <c r="T160" t="s">
-        <v>328</v>
-      </c>
       <c r="U160" t="s">
-        <v>444</v>
+        <v>338</v>
       </c>
     </row>
     <row r="161" spans="1:21">
@@ -11849,11 +11405,8 @@
       <c r="S161" t="s">
         <v>158</v>
       </c>
-      <c r="T161" t="s">
-        <v>329</v>
-      </c>
       <c r="U161" t="s">
-        <v>444</v>
+        <v>339</v>
       </c>
     </row>
     <row r="162" spans="1:21">
@@ -11905,11 +11458,8 @@
       <c r="P162" t="s">
         <v>133</v>
       </c>
-      <c r="T162" t="s">
-        <v>330</v>
-      </c>
       <c r="U162" t="s">
-        <v>444</v>
+        <v>340</v>
       </c>
     </row>
     <row r="163" spans="1:21">
@@ -11970,11 +11520,8 @@
       <c r="S163" t="s">
         <v>163</v>
       </c>
-      <c r="T163" t="s">
-        <v>331</v>
-      </c>
       <c r="U163" t="s">
-        <v>444</v>
+        <v>341</v>
       </c>
     </row>
     <row r="164" spans="1:21">
@@ -12032,11 +11579,8 @@
       <c r="S164" t="s">
         <v>165</v>
       </c>
-      <c r="T164" t="s">
-        <v>332</v>
-      </c>
       <c r="U164" t="s">
-        <v>444</v>
+        <v>342</v>
       </c>
     </row>
     <row r="165" spans="1:21">
@@ -12094,11 +11638,8 @@
       <c r="S165" t="s">
         <v>165</v>
       </c>
-      <c r="T165" t="s">
-        <v>333</v>
-      </c>
       <c r="U165" t="s">
-        <v>444</v>
+        <v>343</v>
       </c>
     </row>
     <row r="166" spans="1:21">
@@ -12156,11 +11697,8 @@
       <c r="S166" t="s">
         <v>160</v>
       </c>
-      <c r="T166" t="s">
-        <v>334</v>
-      </c>
       <c r="U166" t="s">
-        <v>444</v>
+        <v>344</v>
       </c>
     </row>
     <row r="167" spans="1:21">
@@ -12218,11 +11756,8 @@
       <c r="S167" t="s">
         <v>160</v>
       </c>
-      <c r="T167" t="s">
-        <v>335</v>
-      </c>
       <c r="U167" t="s">
-        <v>444</v>
+        <v>345</v>
       </c>
     </row>
     <row r="168" spans="1:21">
@@ -12280,11 +11815,8 @@
       <c r="S168" t="s">
         <v>162</v>
       </c>
-      <c r="T168" t="s">
-        <v>336</v>
-      </c>
       <c r="U168" t="s">
-        <v>444</v>
+        <v>346</v>
       </c>
     </row>
     <row r="169" spans="1:21">
@@ -12342,11 +11874,8 @@
       <c r="S169" t="s">
         <v>165</v>
       </c>
-      <c r="T169" t="s">
-        <v>337</v>
-      </c>
       <c r="U169" t="s">
-        <v>444</v>
+        <v>347</v>
       </c>
     </row>
     <row r="170" spans="1:21">
@@ -12404,11 +11933,8 @@
       <c r="S170" t="s">
         <v>160</v>
       </c>
-      <c r="T170" t="s">
-        <v>338</v>
-      </c>
       <c r="U170" t="s">
-        <v>444</v>
+        <v>348</v>
       </c>
     </row>
     <row r="171" spans="1:21">
@@ -12466,11 +11992,8 @@
       <c r="S171" t="s">
         <v>160</v>
       </c>
-      <c r="T171" t="s">
-        <v>339</v>
-      </c>
       <c r="U171" t="s">
-        <v>444</v>
+        <v>349</v>
       </c>
     </row>
     <row r="172" spans="1:21">
@@ -12528,11 +12051,8 @@
       <c r="S172" t="s">
         <v>160</v>
       </c>
-      <c r="T172" t="s">
-        <v>340</v>
-      </c>
       <c r="U172" t="s">
-        <v>444</v>
+        <v>350</v>
       </c>
     </row>
     <row r="173" spans="1:21">
@@ -12590,11 +12110,8 @@
       <c r="S173" t="s">
         <v>158</v>
       </c>
-      <c r="T173" t="s">
-        <v>341</v>
-      </c>
       <c r="U173" t="s">
-        <v>444</v>
+        <v>351</v>
       </c>
     </row>
     <row r="174" spans="1:21">
@@ -12652,11 +12169,8 @@
       <c r="S174" t="s">
         <v>158</v>
       </c>
-      <c r="T174" t="s">
-        <v>342</v>
-      </c>
       <c r="U174" t="s">
-        <v>444</v>
+        <v>352</v>
       </c>
     </row>
     <row r="175" spans="1:21">
@@ -12705,11 +12219,8 @@
       <c r="O175" t="s">
         <v>104</v>
       </c>
-      <c r="T175" t="s">
-        <v>343</v>
-      </c>
       <c r="U175" t="s">
-        <v>444</v>
+        <v>353</v>
       </c>
     </row>
     <row r="176" spans="1:21">
@@ -12767,11 +12278,8 @@
       <c r="S176" t="s">
         <v>160</v>
       </c>
-      <c r="T176" t="s">
-        <v>344</v>
-      </c>
       <c r="U176" t="s">
-        <v>444</v>
+        <v>354</v>
       </c>
     </row>
     <row r="177" spans="1:21">
@@ -12820,11 +12328,8 @@
       <c r="O177" t="s">
         <v>106</v>
       </c>
-      <c r="T177" t="s">
-        <v>345</v>
-      </c>
       <c r="U177" t="s">
-        <v>444</v>
+        <v>355</v>
       </c>
     </row>
     <row r="178" spans="1:21">
@@ -12879,11 +12384,8 @@
       <c r="R178" t="s">
         <v>151</v>
       </c>
-      <c r="T178" t="s">
-        <v>346</v>
-      </c>
       <c r="U178" t="s">
-        <v>444</v>
+        <v>356</v>
       </c>
     </row>
     <row r="179" spans="1:21">
@@ -12932,11 +12434,8 @@
       <c r="O179" t="s">
         <v>108</v>
       </c>
-      <c r="T179" t="s">
-        <v>347</v>
-      </c>
       <c r="U179" t="s">
-        <v>444</v>
+        <v>357</v>
       </c>
     </row>
     <row r="180" spans="1:21">
@@ -12994,11 +12493,8 @@
       <c r="S180" t="s">
         <v>158</v>
       </c>
-      <c r="T180" t="s">
-        <v>348</v>
-      </c>
       <c r="U180" t="s">
-        <v>444</v>
+        <v>358</v>
       </c>
     </row>
     <row r="181" spans="1:21">
@@ -13047,11 +12543,8 @@
       <c r="O181" t="s">
         <v>61</v>
       </c>
-      <c r="T181" t="s">
-        <v>349</v>
-      </c>
       <c r="U181" t="s">
-        <v>444</v>
+        <v>359</v>
       </c>
     </row>
     <row r="182" spans="1:21">
@@ -13103,11 +12596,8 @@
       <c r="P182" t="s">
         <v>131</v>
       </c>
-      <c r="T182" t="s">
-        <v>350</v>
-      </c>
       <c r="U182" t="s">
-        <v>444</v>
+        <v>360</v>
       </c>
     </row>
     <row r="183" spans="1:21">
@@ -13165,11 +12655,8 @@
       <c r="S183" t="s">
         <v>165</v>
       </c>
-      <c r="T183" t="s">
-        <v>351</v>
-      </c>
       <c r="U183" t="s">
-        <v>444</v>
+        <v>361</v>
       </c>
     </row>
     <row r="184" spans="1:21">
@@ -13227,11 +12714,8 @@
       <c r="S184" t="s">
         <v>155</v>
       </c>
-      <c r="T184" t="s">
-        <v>352</v>
-      </c>
       <c r="U184" t="s">
-        <v>444</v>
+        <v>362</v>
       </c>
     </row>
     <row r="185" spans="1:21">
@@ -13289,11 +12773,8 @@
       <c r="S185" t="s">
         <v>155</v>
       </c>
-      <c r="T185" t="s">
-        <v>353</v>
-      </c>
       <c r="U185" t="s">
-        <v>444</v>
+        <v>363</v>
       </c>
     </row>
     <row r="186" spans="1:21">
@@ -13342,11 +12823,8 @@
       <c r="O186" t="s">
         <v>114</v>
       </c>
-      <c r="T186" t="s">
-        <v>354</v>
-      </c>
       <c r="U186" t="s">
-        <v>444</v>
+        <v>364</v>
       </c>
     </row>
     <row r="187" spans="1:21">
@@ -13395,11 +12873,8 @@
       <c r="O187" t="s">
         <v>116</v>
       </c>
-      <c r="T187" t="s">
-        <v>355</v>
-      </c>
       <c r="U187" t="s">
-        <v>444</v>
+        <v>365</v>
       </c>
     </row>
     <row r="188" spans="1:21">
@@ -13454,11 +12929,8 @@
       <c r="S188" t="s">
         <v>160</v>
       </c>
-      <c r="T188" t="s">
-        <v>356</v>
-      </c>
       <c r="U188" t="s">
-        <v>444</v>
+        <v>366</v>
       </c>
     </row>
     <row r="189" spans="1:21">
@@ -13513,11 +12985,8 @@
       <c r="S189" t="s">
         <v>165</v>
       </c>
-      <c r="T189" t="s">
-        <v>357</v>
-      </c>
       <c r="U189" t="s">
-        <v>444</v>
+        <v>367</v>
       </c>
     </row>
     <row r="190" spans="1:21">
@@ -13566,11 +13035,8 @@
       <c r="O190" t="s">
         <v>118</v>
       </c>
-      <c r="T190" t="s">
-        <v>358</v>
-      </c>
       <c r="U190" t="s">
-        <v>444</v>
+        <v>368</v>
       </c>
     </row>
     <row r="191" spans="1:21">
@@ -13622,11 +13088,8 @@
       <c r="R191" t="s">
         <v>150</v>
       </c>
-      <c r="T191" t="s">
-        <v>235</v>
-      </c>
       <c r="U191" t="s">
-        <v>444</v>
+        <v>245</v>
       </c>
     </row>
     <row r="192" spans="1:21">
@@ -13681,11 +13144,8 @@
       <c r="S192" t="s">
         <v>161</v>
       </c>
-      <c r="T192" t="s">
-        <v>359</v>
-      </c>
       <c r="U192" t="s">
-        <v>444</v>
+        <v>369</v>
       </c>
     </row>
     <row r="193" spans="1:21">
@@ -13734,11 +13194,8 @@
       <c r="O193" t="s">
         <v>123</v>
       </c>
-      <c r="T193" t="s">
-        <v>360</v>
-      </c>
       <c r="U193" t="s">
-        <v>444</v>
+        <v>370</v>
       </c>
     </row>
     <row r="194" spans="1:21">
@@ -13793,11 +13250,8 @@
       <c r="Q194" t="s">
         <v>143</v>
       </c>
-      <c r="T194" t="s">
-        <v>361</v>
-      </c>
       <c r="U194" t="s">
-        <v>444</v>
+        <v>371</v>
       </c>
     </row>
     <row r="195" spans="1:21">
@@ -13858,11 +13312,8 @@
       <c r="S195" t="s">
         <v>155</v>
       </c>
-      <c r="T195" t="s">
-        <v>362</v>
-      </c>
       <c r="U195" t="s">
-        <v>444</v>
+        <v>372</v>
       </c>
     </row>
     <row r="196" spans="1:21">
@@ -13914,11 +13365,8 @@
       <c r="P196" t="s">
         <v>131</v>
       </c>
-      <c r="T196" t="s">
-        <v>363</v>
-      </c>
       <c r="U196" t="s">
-        <v>444</v>
+        <v>373</v>
       </c>
     </row>
     <row r="197" spans="1:21">
@@ -13973,11 +13421,8 @@
       <c r="S197" t="s">
         <v>162</v>
       </c>
-      <c r="T197" t="s">
-        <v>364</v>
-      </c>
       <c r="U197" t="s">
-        <v>444</v>
+        <v>374</v>
       </c>
     </row>
     <row r="198" spans="1:21">
@@ -14029,11 +13474,8 @@
       <c r="P198" t="s">
         <v>137</v>
       </c>
-      <c r="T198" t="s">
-        <v>365</v>
-      </c>
       <c r="U198" t="s">
-        <v>444</v>
+        <v>375</v>
       </c>
     </row>
     <row r="199" spans="1:21">
@@ -14094,11 +13536,8 @@
       <c r="S199" t="s">
         <v>158</v>
       </c>
-      <c r="T199" t="s">
-        <v>366</v>
-      </c>
       <c r="U199" t="s">
-        <v>444</v>
+        <v>376</v>
       </c>
     </row>
     <row r="200" spans="1:21">
@@ -14159,11 +13598,8 @@
       <c r="S200" t="s">
         <v>166</v>
       </c>
-      <c r="T200" t="s">
-        <v>367</v>
-      </c>
       <c r="U200" t="s">
-        <v>444</v>
+        <v>377</v>
       </c>
     </row>
     <row r="201" spans="1:21">
@@ -14224,11 +13660,8 @@
       <c r="S201" t="s">
         <v>155</v>
       </c>
-      <c r="T201" t="s">
-        <v>368</v>
-      </c>
       <c r="U201" t="s">
-        <v>444</v>
+        <v>378</v>
       </c>
     </row>
     <row r="202" spans="1:21">
@@ -14289,11 +13722,8 @@
       <c r="S202" t="s">
         <v>167</v>
       </c>
-      <c r="T202" t="s">
-        <v>369</v>
-      </c>
       <c r="U202" t="s">
-        <v>444</v>
+        <v>379</v>
       </c>
     </row>
     <row r="203" spans="1:21">
@@ -14345,11 +13775,8 @@
       <c r="P203" t="s">
         <v>136</v>
       </c>
-      <c r="T203" t="s">
-        <v>370</v>
-      </c>
       <c r="U203" t="s">
-        <v>444</v>
+        <v>380</v>
       </c>
     </row>
     <row r="204" spans="1:21">
@@ -14410,11 +13837,8 @@
       <c r="S204" t="s">
         <v>156</v>
       </c>
-      <c r="T204" t="s">
-        <v>371</v>
-      </c>
       <c r="U204" t="s">
-        <v>444</v>
+        <v>381</v>
       </c>
     </row>
     <row r="205" spans="1:21">
@@ -14472,11 +13896,8 @@
       <c r="S205" t="s">
         <v>165</v>
       </c>
-      <c r="T205" t="s">
-        <v>372</v>
-      </c>
       <c r="U205" t="s">
-        <v>444</v>
+        <v>382</v>
       </c>
     </row>
     <row r="206" spans="1:21">
@@ -14534,11 +13955,8 @@
       <c r="S206" t="s">
         <v>163</v>
       </c>
-      <c r="T206" t="s">
-        <v>373</v>
-      </c>
       <c r="U206" t="s">
-        <v>444</v>
+        <v>383</v>
       </c>
     </row>
     <row r="207" spans="1:21">
@@ -14599,11 +14017,8 @@
       <c r="S207" t="s">
         <v>155</v>
       </c>
-      <c r="T207" t="s">
-        <v>374</v>
-      </c>
       <c r="U207" t="s">
-        <v>444</v>
+        <v>384</v>
       </c>
     </row>
     <row r="208" spans="1:21">
@@ -14661,11 +14076,8 @@
       <c r="S208" t="s">
         <v>158</v>
       </c>
-      <c r="T208" t="s">
-        <v>375</v>
-      </c>
       <c r="U208" t="s">
-        <v>444</v>
+        <v>385</v>
       </c>
     </row>
     <row r="209" spans="1:21">
@@ -14723,11 +14135,8 @@
       <c r="S209" t="s">
         <v>158</v>
       </c>
-      <c r="T209" t="s">
-        <v>376</v>
-      </c>
       <c r="U209" t="s">
-        <v>444</v>
+        <v>386</v>
       </c>
     </row>
     <row r="210" spans="1:21">
@@ -14785,11 +14194,8 @@
       <c r="S210" t="s">
         <v>165</v>
       </c>
-      <c r="T210" t="s">
-        <v>377</v>
-      </c>
       <c r="U210" t="s">
-        <v>444</v>
+        <v>387</v>
       </c>
     </row>
     <row r="211" spans="1:21">
@@ -14838,11 +14244,8 @@
       <c r="O211" t="s">
         <v>96</v>
       </c>
-      <c r="T211" t="s">
-        <v>378</v>
-      </c>
       <c r="U211" t="s">
-        <v>444</v>
+        <v>388</v>
       </c>
     </row>
     <row r="212" spans="1:21">
@@ -14903,11 +14306,8 @@
       <c r="S212" t="s">
         <v>155</v>
       </c>
-      <c r="T212" t="s">
-        <v>379</v>
-      </c>
       <c r="U212" t="s">
-        <v>444</v>
+        <v>389</v>
       </c>
     </row>
     <row r="213" spans="1:21">
@@ -14956,11 +14356,8 @@
       <c r="O213" t="s">
         <v>60</v>
       </c>
-      <c r="T213" t="s">
-        <v>380</v>
-      </c>
       <c r="U213" t="s">
-        <v>444</v>
+        <v>390</v>
       </c>
     </row>
     <row r="214" spans="1:21">
@@ -15018,11 +14415,8 @@
       <c r="S214" t="s">
         <v>162</v>
       </c>
-      <c r="T214" t="s">
-        <v>381</v>
-      </c>
       <c r="U214" t="s">
-        <v>444</v>
+        <v>391</v>
       </c>
     </row>
     <row r="215" spans="1:21">
@@ -15080,11 +14474,8 @@
       <c r="S215" t="s">
         <v>165</v>
       </c>
-      <c r="T215" t="s">
-        <v>382</v>
-      </c>
       <c r="U215" t="s">
-        <v>444</v>
+        <v>392</v>
       </c>
     </row>
     <row r="216" spans="1:21">
@@ -15136,11 +14527,8 @@
       <c r="P216" t="s">
         <v>140</v>
       </c>
-      <c r="T216" t="s">
-        <v>383</v>
-      </c>
       <c r="U216" t="s">
-        <v>444</v>
+        <v>393</v>
       </c>
     </row>
     <row r="217" spans="1:21">
@@ -15198,11 +14586,8 @@
       <c r="S217" t="s">
         <v>165</v>
       </c>
-      <c r="T217" t="s">
-        <v>384</v>
-      </c>
       <c r="U217" t="s">
-        <v>444</v>
+        <v>394</v>
       </c>
     </row>
     <row r="218" spans="1:21">
@@ -15260,11 +14645,8 @@
       <c r="S218" t="s">
         <v>155</v>
       </c>
-      <c r="T218" t="s">
-        <v>385</v>
-      </c>
       <c r="U218" t="s">
-        <v>444</v>
+        <v>395</v>
       </c>
     </row>
     <row r="219" spans="1:21">
@@ -15313,11 +14695,8 @@
       <c r="O219" t="s">
         <v>115</v>
       </c>
-      <c r="T219" t="s">
-        <v>386</v>
-      </c>
       <c r="U219" t="s">
-        <v>444</v>
+        <v>396</v>
       </c>
     </row>
     <row r="220" spans="1:21">
@@ -15375,11 +14754,8 @@
       <c r="S220" t="s">
         <v>160</v>
       </c>
-      <c r="T220" t="s">
-        <v>387</v>
-      </c>
       <c r="U220" t="s">
-        <v>444</v>
+        <v>397</v>
       </c>
     </row>
     <row r="221" spans="1:21">
@@ -15434,11 +14810,8 @@
       <c r="S221" t="s">
         <v>155</v>
       </c>
-      <c r="T221" t="s">
-        <v>388</v>
-      </c>
       <c r="U221" t="s">
-        <v>444</v>
+        <v>398</v>
       </c>
     </row>
     <row r="222" spans="1:21">
@@ -15493,11 +14866,8 @@
       <c r="S222" t="s">
         <v>158</v>
       </c>
-      <c r="T222" t="s">
-        <v>389</v>
-      </c>
       <c r="U222" t="s">
-        <v>444</v>
+        <v>399</v>
       </c>
     </row>
     <row r="223" spans="1:21">
@@ -15552,11 +14922,8 @@
       <c r="S223" t="s">
         <v>155</v>
       </c>
-      <c r="T223" t="s">
-        <v>390</v>
-      </c>
       <c r="U223" t="s">
-        <v>444</v>
+        <v>400</v>
       </c>
     </row>
     <row r="224" spans="1:21">
@@ -15605,11 +14972,8 @@
       <c r="O224" t="s">
         <v>124</v>
       </c>
-      <c r="T224" t="s">
-        <v>391</v>
-      </c>
       <c r="U224" t="s">
-        <v>444</v>
+        <v>401</v>
       </c>
     </row>
     <row r="225" spans="1:21">
@@ -15670,11 +15034,8 @@
       <c r="S225" t="s">
         <v>155</v>
       </c>
-      <c r="T225" t="s">
-        <v>392</v>
-      </c>
       <c r="U225" t="s">
-        <v>444</v>
+        <v>402</v>
       </c>
     </row>
     <row r="226" spans="1:21">
@@ -15735,11 +15096,8 @@
       <c r="S226" t="s">
         <v>162</v>
       </c>
-      <c r="T226" t="s">
-        <v>393</v>
-      </c>
       <c r="U226" t="s">
-        <v>444</v>
+        <v>403</v>
       </c>
     </row>
     <row r="227" spans="1:21">
@@ -15800,11 +15158,8 @@
       <c r="S227" t="s">
         <v>157</v>
       </c>
-      <c r="T227" t="s">
-        <v>394</v>
-      </c>
       <c r="U227" t="s">
-        <v>444</v>
+        <v>404</v>
       </c>
     </row>
     <row r="228" spans="1:21">
@@ -15865,11 +15220,8 @@
       <c r="S228" t="s">
         <v>155</v>
       </c>
-      <c r="T228" t="s">
-        <v>395</v>
-      </c>
       <c r="U228" t="s">
-        <v>444</v>
+        <v>405</v>
       </c>
     </row>
     <row r="229" spans="1:21">
@@ -15930,11 +15282,8 @@
       <c r="S229" t="s">
         <v>160</v>
       </c>
-      <c r="T229" t="s">
-        <v>396</v>
-      </c>
       <c r="U229" t="s">
-        <v>444</v>
+        <v>406</v>
       </c>
     </row>
     <row r="230" spans="1:21">
@@ -15995,11 +15344,8 @@
       <c r="S230" t="s">
         <v>165</v>
       </c>
-      <c r="T230" t="s">
-        <v>397</v>
-      </c>
       <c r="U230" t="s">
-        <v>444</v>
+        <v>407</v>
       </c>
     </row>
     <row r="231" spans="1:21">
@@ -16054,11 +15400,8 @@
       <c r="S231" t="s">
         <v>158</v>
       </c>
-      <c r="T231" t="s">
-        <v>398</v>
-      </c>
       <c r="U231" t="s">
-        <v>444</v>
+        <v>408</v>
       </c>
     </row>
     <row r="232" spans="1:21">
@@ -16116,11 +15459,8 @@
       <c r="S232" t="s">
         <v>165</v>
       </c>
-      <c r="T232" t="s">
-        <v>399</v>
-      </c>
       <c r="U232" t="s">
-        <v>444</v>
+        <v>409</v>
       </c>
     </row>
     <row r="233" spans="1:21">
@@ -16178,11 +15518,8 @@
       <c r="S233" t="s">
         <v>160</v>
       </c>
-      <c r="T233" t="s">
-        <v>400</v>
-      </c>
       <c r="U233" t="s">
-        <v>444</v>
+        <v>410</v>
       </c>
     </row>
     <row r="234" spans="1:21">
@@ -16237,11 +15574,8 @@
       <c r="Q234" t="s">
         <v>144</v>
       </c>
-      <c r="T234" t="s">
-        <v>401</v>
-      </c>
       <c r="U234" t="s">
-        <v>444</v>
+        <v>411</v>
       </c>
     </row>
     <row r="235" spans="1:21">
@@ -16299,11 +15633,8 @@
       <c r="S235" t="s">
         <v>158</v>
       </c>
-      <c r="T235" t="s">
-        <v>402</v>
-      </c>
       <c r="U235" t="s">
-        <v>444</v>
+        <v>412</v>
       </c>
     </row>
     <row r="236" spans="1:21">
@@ -16361,11 +15692,8 @@
       <c r="S236" t="s">
         <v>159</v>
       </c>
-      <c r="T236" t="s">
-        <v>403</v>
-      </c>
       <c r="U236" t="s">
-        <v>444</v>
+        <v>413</v>
       </c>
     </row>
     <row r="237" spans="1:21">
@@ -16414,11 +15742,8 @@
       <c r="O237" t="s">
         <v>107</v>
       </c>
-      <c r="T237" t="s">
-        <v>404</v>
-      </c>
       <c r="U237" t="s">
-        <v>444</v>
+        <v>414</v>
       </c>
     </row>
     <row r="238" spans="1:21">
@@ -16476,11 +15801,8 @@
       <c r="S238" t="s">
         <v>165</v>
       </c>
-      <c r="T238" t="s">
-        <v>405</v>
-      </c>
       <c r="U238" t="s">
-        <v>444</v>
+        <v>415</v>
       </c>
     </row>
     <row r="239" spans="1:21">
@@ -16529,11 +15851,8 @@
       <c r="O239" t="s">
         <v>62</v>
       </c>
-      <c r="T239" t="s">
-        <v>406</v>
-      </c>
       <c r="U239" t="s">
-        <v>444</v>
+        <v>416</v>
       </c>
     </row>
     <row r="240" spans="1:21">
@@ -16582,11 +15901,8 @@
       <c r="O240" t="s">
         <v>111</v>
       </c>
-      <c r="T240" t="s">
-        <v>407</v>
-      </c>
       <c r="U240" t="s">
-        <v>444</v>
+        <v>417</v>
       </c>
     </row>
     <row r="241" spans="1:21">
@@ -16635,11 +15951,8 @@
       <c r="O241" t="s">
         <v>64</v>
       </c>
-      <c r="T241" t="s">
-        <v>408</v>
-      </c>
       <c r="U241" t="s">
-        <v>444</v>
+        <v>418</v>
       </c>
     </row>
     <row r="242" spans="1:21">
@@ -16694,11 +16007,8 @@
       <c r="S242" t="s">
         <v>160</v>
       </c>
-      <c r="T242" t="s">
-        <v>409</v>
-      </c>
       <c r="U242" t="s">
-        <v>444</v>
+        <v>419</v>
       </c>
     </row>
     <row r="243" spans="1:21">
@@ -16750,11 +16060,8 @@
       <c r="R243" t="s">
         <v>152</v>
       </c>
-      <c r="T243" t="s">
-        <v>410</v>
-      </c>
       <c r="U243" t="s">
-        <v>444</v>
+        <v>420</v>
       </c>
     </row>
     <row r="244" spans="1:21">
@@ -16809,11 +16116,8 @@
       <c r="S244" t="s">
         <v>155</v>
       </c>
-      <c r="T244" t="s">
-        <v>411</v>
-      </c>
       <c r="U244" t="s">
-        <v>444</v>
+        <v>421</v>
       </c>
     </row>
     <row r="245" spans="1:21">
@@ -16874,11 +16178,8 @@
       <c r="S245" t="s">
         <v>157</v>
       </c>
-      <c r="T245" t="s">
-        <v>412</v>
-      </c>
       <c r="U245" t="s">
-        <v>444</v>
+        <v>422</v>
       </c>
     </row>
     <row r="246" spans="1:21">
@@ -16930,11 +16231,8 @@
       <c r="P246" t="s">
         <v>137</v>
       </c>
-      <c r="T246" t="s">
-        <v>413</v>
-      </c>
       <c r="U246" t="s">
-        <v>444</v>
+        <v>423</v>
       </c>
     </row>
     <row r="247" spans="1:21">
@@ -16995,11 +16293,8 @@
       <c r="S247" t="s">
         <v>157</v>
       </c>
-      <c r="T247" t="s">
-        <v>414</v>
-      </c>
       <c r="U247" t="s">
-        <v>444</v>
+        <v>424</v>
       </c>
     </row>
     <row r="248" spans="1:21">
@@ -17057,11 +16352,8 @@
       <c r="S248" t="s">
         <v>161</v>
       </c>
-      <c r="T248" t="s">
-        <v>415</v>
-      </c>
       <c r="U248" t="s">
-        <v>444</v>
+        <v>425</v>
       </c>
     </row>
     <row r="249" spans="1:21">
@@ -17122,11 +16414,8 @@
       <c r="S249" t="s">
         <v>157</v>
       </c>
-      <c r="T249" t="s">
-        <v>416</v>
-      </c>
       <c r="U249" t="s">
-        <v>444</v>
+        <v>426</v>
       </c>
     </row>
     <row r="250" spans="1:21">
@@ -17184,11 +16473,8 @@
       <c r="S250" t="s">
         <v>160</v>
       </c>
-      <c r="T250" t="s">
-        <v>417</v>
-      </c>
       <c r="U250" t="s">
-        <v>444</v>
+        <v>427</v>
       </c>
     </row>
     <row r="251" spans="1:21">
@@ -17243,11 +16529,8 @@
       <c r="R251" t="s">
         <v>151</v>
       </c>
-      <c r="T251" t="s">
-        <v>418</v>
-      </c>
       <c r="U251" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
     </row>
     <row r="252" spans="1:21">
@@ -17302,11 +16585,8 @@
       <c r="S252" t="s">
         <v>160</v>
       </c>
-      <c r="T252" t="s">
-        <v>419</v>
-      </c>
       <c r="U252" t="s">
-        <v>444</v>
+        <v>429</v>
       </c>
     </row>
     <row r="253" spans="1:21">
@@ -17358,11 +16638,8 @@
       <c r="P253" t="s">
         <v>136</v>
       </c>
-      <c r="T253" t="s">
-        <v>420</v>
-      </c>
       <c r="U253" t="s">
-        <v>444</v>
+        <v>430</v>
       </c>
     </row>
     <row r="254" spans="1:21">
@@ -17420,11 +16697,8 @@
       <c r="R254" t="s">
         <v>150</v>
       </c>
-      <c r="T254" t="s">
-        <v>421</v>
-      </c>
       <c r="U254" t="s">
-        <v>444</v>
+        <v>431</v>
       </c>
     </row>
     <row r="255" spans="1:21">
@@ -17485,11 +16759,8 @@
       <c r="S255" t="s">
         <v>156</v>
       </c>
-      <c r="T255" t="s">
-        <v>422</v>
-      </c>
       <c r="U255" t="s">
-        <v>444</v>
+        <v>432</v>
       </c>
     </row>
     <row r="256" spans="1:21">
@@ -17547,11 +16818,8 @@
       <c r="S256" t="s">
         <v>165</v>
       </c>
-      <c r="T256" t="s">
-        <v>423</v>
-      </c>
       <c r="U256" t="s">
-        <v>444</v>
+        <v>433</v>
       </c>
     </row>
     <row r="257" spans="1:21">
@@ -17609,11 +16877,8 @@
       <c r="S257" t="s">
         <v>165</v>
       </c>
-      <c r="T257" t="s">
-        <v>424</v>
-      </c>
       <c r="U257" t="s">
-        <v>444</v>
+        <v>434</v>
       </c>
     </row>
     <row r="258" spans="1:21">
@@ -17671,11 +16936,8 @@
       <c r="S258" t="s">
         <v>162</v>
       </c>
-      <c r="T258" t="s">
-        <v>425</v>
-      </c>
       <c r="U258" t="s">
-        <v>444</v>
+        <v>435</v>
       </c>
     </row>
     <row r="259" spans="1:21">
@@ -17736,11 +16998,8 @@
       <c r="S259" t="s">
         <v>157</v>
       </c>
-      <c r="T259" t="s">
-        <v>426</v>
-      </c>
       <c r="U259" t="s">
-        <v>444</v>
+        <v>436</v>
       </c>
     </row>
     <row r="260" spans="1:21">
@@ -17798,11 +17057,8 @@
       <c r="S260" t="s">
         <v>165</v>
       </c>
-      <c r="T260" t="s">
-        <v>427</v>
-      </c>
       <c r="U260" t="s">
-        <v>444</v>
+        <v>437</v>
       </c>
     </row>
     <row r="261" spans="1:21">
@@ -17854,11 +17110,8 @@
       <c r="P261" t="s">
         <v>131</v>
       </c>
-      <c r="T261" t="s">
-        <v>428</v>
-      </c>
       <c r="U261" t="s">
-        <v>444</v>
+        <v>438</v>
       </c>
     </row>
     <row r="262" spans="1:21">
@@ -17910,11 +17163,8 @@
       <c r="P262" t="s">
         <v>138</v>
       </c>
-      <c r="T262" t="s">
-        <v>429</v>
-      </c>
       <c r="U262" t="s">
-        <v>444</v>
+        <v>439</v>
       </c>
     </row>
     <row r="263" spans="1:21">
@@ -17972,11 +17222,8 @@
       <c r="S263" t="s">
         <v>157</v>
       </c>
-      <c r="T263" t="s">
-        <v>430</v>
-      </c>
       <c r="U263" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
     </row>
     <row r="264" spans="1:21">
@@ -18028,11 +17275,8 @@
       <c r="P264" t="s">
         <v>137</v>
       </c>
-      <c r="T264" t="s">
-        <v>431</v>
-      </c>
       <c r="U264" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="265" spans="1:21">
@@ -18090,11 +17334,8 @@
       <c r="S265" t="s">
         <v>160</v>
       </c>
-      <c r="T265" t="s">
-        <v>432</v>
-      </c>
       <c r="U265" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="266" spans="1:21">
@@ -18152,11 +17393,8 @@
       <c r="S266" t="s">
         <v>165</v>
       </c>
-      <c r="T266" t="s">
-        <v>433</v>
-      </c>
       <c r="U266" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
     </row>
     <row r="267" spans="1:21">
@@ -18205,9 +17443,6 @@
       <c r="O267" t="s">
         <v>112</v>
       </c>
-      <c r="T267" t="s">
-        <v>434</v>
-      </c>
       <c r="U267" t="s">
         <v>444</v>
       </c>
@@ -18267,11 +17502,8 @@
       <c r="S268" t="s">
         <v>158</v>
       </c>
-      <c r="T268" t="s">
-        <v>435</v>
-      </c>
       <c r="U268" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
     </row>
     <row r="269" spans="1:21">
@@ -18326,11 +17558,8 @@
       <c r="S269" t="s">
         <v>162</v>
       </c>
-      <c r="T269" t="s">
-        <v>436</v>
-      </c>
       <c r="U269" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
     </row>
     <row r="270" spans="1:21">
@@ -18379,11 +17608,8 @@
       <c r="O270" t="s">
         <v>122</v>
       </c>
-      <c r="T270" t="s">
-        <v>437</v>
-      </c>
       <c r="U270" t="s">
-        <v>444</v>
+        <v>447</v>
       </c>
     </row>
   </sheetData>

</xml_diff>